<commit_message>
fixed tail - again - geometry is hard
</commit_message>
<xml_diff>
--- a/CAD and Drawings/Solidworks/Airfoil Curves/0012VTail.xlsx
+++ b/CAD and Drawings/Solidworks/Airfoil Curves/0012VTail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grega\Documents\NACA0012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5607F396-8B8A-4EB9-A747-DD2172BCA8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ABC2E88-D887-4C14-9994-E319CCA5160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D9CF6ABE-F6CA-4256-B073-D59D38990502}"/>
   </bookViews>
@@ -1205,8 +1205,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection sqref="A1:C66"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1217,11 +1217,11 @@
         <v>48</v>
       </c>
       <c r="B1">
-        <f>18*Upper.dat!B1*COS(RADIANS(26))</f>
+        <f>18*Upper.dat!B1*COS(RADIANS(47))</f>
         <v>0</v>
       </c>
       <c r="C1">
-        <f>-Upper.dat!B1*SIN(RADIANS(26))+4</f>
+        <f>-Upper.dat!B1*SIN(RADIANS(47))+4</f>
         <v>4</v>
       </c>
     </row>
@@ -1231,12 +1231,12 @@
         <v>48.010510199999999</v>
       </c>
       <c r="B2">
-        <f>18*Upper.dat!B2*COS(RADIANS(26))</f>
-        <v>6.8912478361536522E-2</v>
+        <f>18*Upper.dat!B2*COS(RADIANS(47))</f>
+        <v>5.2290285437390172E-2</v>
       </c>
       <c r="C2">
-        <f>-Upper.dat!B2*SIN(RADIANS(26))+4</f>
-        <v>3.9981327299191243</v>
+        <f>-Upper.dat!B2*SIN(RADIANS(47))+4</f>
+        <v>3.9968847518921491</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1245,12 +1245,12 @@
         <v>48.042015599999999</v>
       </c>
       <c r="B3">
-        <f>18*Upper.dat!B3*COS(RADIANS(26))</f>
-        <v>0.13631763061569294</v>
+        <f>18*Upper.dat!B3*COS(RADIANS(47))</f>
+        <v>0.10343682282977998</v>
       </c>
       <c r="C3">
-        <f>-Upper.dat!B3*SIN(RADIANS(26))+4</f>
-        <v>3.9963063027307024</v>
+        <f>-Upper.dat!B3*SIN(RADIANS(47))+4</f>
+        <v>3.993837643762943</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1259,12 +1259,12 @@
         <v>48.094442400000005</v>
       </c>
       <c r="B4">
-        <f>18*Upper.dat!B4*COS(RADIANS(26))</f>
-        <v>0.20213950236321315</v>
+        <f>18*Upper.dat!B4*COS(RADIANS(47))</f>
+        <v>0.15338197853357172</v>
       </c>
       <c r="C4">
-        <f>-Upper.dat!B4*SIN(RADIANS(26))+4</f>
-        <v>3.9945227765144988</v>
+        <f>-Upper.dat!B4*SIN(RADIANS(47))+4</f>
+        <v>3.9908621091966068</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1273,12 +1273,12 @@
         <v>48.167668199999994</v>
       </c>
       <c r="B5">
-        <f>18*Upper.dat!B5*COS(RADIANS(26))</f>
-        <v>0.26627630897485977</v>
+        <f>18*Upper.dat!B5*COS(RADIANS(47))</f>
+        <v>0.20204851911524929</v>
       </c>
       <c r="C5">
-        <f>-Upper.dat!B5*SIN(RADIANS(26))+4</f>
-        <v>3.9927849092527739</v>
+        <f>-Upper.dat!B5*SIN(RADIANS(47))+4</f>
+        <v>3.9879627494552214</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1287,12 +1287,12 @@
         <v>48.261523800000006</v>
       </c>
       <c r="B6">
-        <f>18*Upper.dat!B6*COS(RADIANS(26))</f>
-        <v>0.32860852269936625</v>
+        <f>18*Upper.dat!B6*COS(RADIANS(47))</f>
+        <v>0.24934574778984689</v>
       </c>
       <c r="C6">
-        <f>-Upper.dat!B6*SIN(RADIANS(26))+4</f>
-        <v>3.9910959396999464</v>
+        <f>-Upper.dat!B6*SIN(RADIANS(47))+4</f>
+        <v>3.9851449678940258</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1301,12 +1301,12 @@
         <v>48.375787799999998</v>
       </c>
       <c r="B7">
-        <f>18*Upper.dat!B7*COS(RADIANS(26))</f>
-        <v>0.38899564312026419</v>
+        <f>18*Upper.dat!B7*COS(RADIANS(47))</f>
+        <v>0.29516705386716907</v>
       </c>
       <c r="C7">
-        <f>-Upper.dat!B7*SIN(RADIANS(26))+4</f>
-        <v>3.9894596748911173</v>
+        <f>-Upper.dat!B7*SIN(RADIANS(47))+4</f>
+        <v>3.9824151159557042</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1315,12 +1315,12 @@
         <v>48.510193799999996</v>
       </c>
       <c r="B8">
-        <f>18*Upper.dat!B8*COS(RADIANS(26))</f>
-        <v>0.44728104248987471</v>
+        <f>18*Upper.dat!B8*COS(RADIANS(47))</f>
+        <v>0.33939358935584657</v>
       </c>
       <c r="C8">
-        <f>-Upper.dat!B8*SIN(RADIANS(26))+4</f>
-        <v>3.9878803588516654</v>
+        <f>-Upper.dat!B8*SIN(RADIANS(47))+4</f>
+        <v>3.9797802741328789</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1329,12 +1329,12 @@
         <v>48.664428599999994</v>
       </c>
       <c r="B9">
-        <f>18*Upper.dat!B9*COS(RADIANS(26))</f>
-        <v>0.50329682125562258</v>
+        <f>18*Upper.dat!B9*COS(RADIANS(47))</f>
+        <v>0.38189795330125242</v>
       </c>
       <c r="C9">
-        <f>-Upper.dat!B9*SIN(RADIANS(26))+4</f>
-        <v>3.986362541030668</v>
+        <f>-Upper.dat!B9*SIN(RADIANS(47))+4</f>
+        <v>3.9772480324698485</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1343,12 +1343,12 @@
         <v>48.838130399999997</v>
       </c>
       <c r="B10">
-        <f>18*Upper.dat!B10*COS(RADIANS(26))</f>
-        <v>0.55686542792778515</v>
+        <f>18*Upper.dat!B10*COS(RADIANS(47))</f>
+        <v>0.4225454209293229</v>
       </c>
       <c r="C10">
-        <f>-Upper.dat!B10*SIN(RADIANS(26))+4</f>
-        <v>3.9849110324085526</v>
+        <f>-Upper.dat!B10*SIN(RADIANS(47))+4</f>
+        <v>3.9748264173350658</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1357,12 +1357,12 @@
         <v>49.030895999999998</v>
       </c>
       <c r="B11">
-        <f>18*Upper.dat!B11*COS(RADIANS(26))</f>
-        <v>0.60780612224276487</v>
+        <f>18*Upper.dat!B11*COS(RADIANS(47))</f>
+        <v>0.46119884784765985</v>
       </c>
       <c r="C11">
-        <f>-Upper.dat!B11*SIN(RADIANS(26))+4</f>
-        <v>3.9835307303695755</v>
+        <f>-Upper.dat!B11*SIN(RADIANS(47))+4</f>
+        <v>3.9725235992482633</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1371,12 +1371,12 @@
         <v>49.242273600000004</v>
       </c>
       <c r="B12">
-        <f>18*Upper.dat!B12*COS(RADIANS(26))</f>
-        <v>0.65593336548766734</v>
+        <f>18*Upper.dat!B12*COS(RADIANS(47))</f>
+        <v>0.4977174486355731</v>
       </c>
       <c r="C12">
-        <f>-Upper.dat!B12*SIN(RADIANS(26))+4</f>
-        <v>3.9822266623179989</v>
+        <f>-Upper.dat!B12*SIN(RADIANS(47))+4</f>
+        <v>3.9703479656472163</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1385,12 +1385,12 @@
         <v>49.4717682</v>
       </c>
       <c r="B13">
-        <f>18*Upper.dat!B13*COS(RADIANS(26))</f>
-        <v>0.70107137484845539</v>
+        <f>18*Upper.dat!B13*COS(RADIANS(47))</f>
+        <v>0.53196784057719548</v>
       </c>
       <c r="C13">
-        <f>-Upper.dat!B13*SIN(RADIANS(26))+4</f>
-        <v>3.9810035913097632</v>
+        <f>-Upper.dat!B13*SIN(RADIANS(47))+4</f>
+        <v>3.9683074629458677</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1399,12 +1399,12 @@
         <v>49.718846999999997</v>
       </c>
       <c r="B14">
-        <f>18*Upper.dat!B14*COS(RADIANS(26))</f>
-        <v>0.7430460281481378</v>
+        <f>18*Upper.dat!B14*COS(RADIANS(47))</f>
+        <v>0.56381790103592588</v>
       </c>
       <c r="C14">
-        <f>-Upper.dat!B14*SIN(RADIANS(26))+4</f>
-        <v>3.9798662354037626</v>
+        <f>-Upper.dat!B14*SIN(RADIANS(47))+4</f>
+        <v>3.9664099624876266</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1413,12 +1413,12 @@
         <v>49.982930400000001</v>
       </c>
       <c r="B15">
-        <f>18*Upper.dat!B15*COS(RADIANS(26))</f>
-        <v>0.78170105233192777</v>
+        <f>18*Upper.dat!B15*COS(RADIANS(47))</f>
+        <v>0.5931490511587717</v>
       </c>
       <c r="C15">
-        <f>-Upper.dat!B15*SIN(RADIANS(26))+4</f>
-        <v>3.9788188290145272</v>
+        <f>-Upper.dat!B15*SIN(RADIANS(47))+4</f>
+        <v>3.964662528730917</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1427,12 +1427,12 @@
         <v>50.263402799999994</v>
       </c>
       <c r="B16">
-        <f>18*Upper.dat!B16*COS(RADIANS(26))</f>
-        <v>0.81688830426075287</v>
+        <f>18*Upper.dat!B16*COS(RADIANS(47))</f>
+        <v>0.61984888101342672</v>
       </c>
       <c r="C16">
-        <f>-Upper.dat!B16*SIN(RADIANS(26))+4</f>
-        <v>3.977865386266318</v>
+        <f>-Upper.dat!B16*SIN(RADIANS(47))+4</f>
+        <v>3.9630718586142994</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1441,12 +1441,12 @@
         <v>50.559608999999995</v>
       </c>
       <c r="B17">
-        <f>18*Upper.dat!B17*COS(RADIANS(26))</f>
-        <v>0.84848557091030152</v>
+        <f>18*Upper.dat!B17*COS(RADIANS(47))</f>
+        <v>0.64382465624934426</v>
       </c>
       <c r="C17">
-        <f>-Upper.dat!B17*SIN(RADIANS(26))+4</f>
-        <v>3.9770092186743966</v>
+        <f>-Upper.dat!B17*SIN(RADIANS(47))+4</f>
+        <v>3.9616434768831001</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1455,12 +1455,12 @@
         <v>50.870857799999996</v>
       </c>
       <c r="B18">
-        <f>18*Upper.dat!B18*COS(RADIANS(26))</f>
-        <v>0.87638685831839436</v>
+        <f>18*Upper.dat!B18*COS(RADIANS(47))</f>
+        <v>0.66499594942190499</v>
       </c>
       <c r="C18">
-        <f>-Upper.dat!B18*SIN(RADIANS(26))+4</f>
-        <v>3.9762531982781817</v>
+        <f>-Upper.dat!B18*SIN(RADIANS(47))+4</f>
+        <v>3.9603821750859329</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1469,12 +1469,12 @@
         <v>51.196420200000006</v>
       </c>
       <c r="B19">
-        <f>18*Upper.dat!B19*COS(RADIANS(26))</f>
-        <v>0.90051371842843086</v>
+        <f>18*Upper.dat!B19*COS(RADIANS(47))</f>
+        <v>0.68330323471852483</v>
       </c>
       <c r="C19">
-        <f>-Upper.dat!B19*SIN(RADIANS(26))+4</f>
-        <v>3.9755994507262127</v>
+        <f>-Upper.dat!B19*SIN(RADIANS(47))+4</f>
+        <v>3.9592914995349555</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1483,12 +1483,12 @@
         <v>51.5355366</v>
       </c>
       <c r="B20">
-        <f>18*Upper.dat!B20*COS(RADIANS(26))</f>
-        <v>0.92081200527696394</v>
+        <f>18*Upper.dat!B20*COS(RADIANS(47))</f>
+        <v>0.69870542657747037</v>
       </c>
       <c r="C20">
-        <f>-Upper.dat!B20*SIN(RADIANS(26))+4</f>
-        <v>3.975049443171319</v>
+        <f>-Upper.dat!B20*SIN(RADIANS(47))+4</f>
+        <v>3.958373897945215</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1497,12 +1497,12 @@
         <v>51.887416799999997</v>
       </c>
       <c r="B21">
-        <f>18*Upper.dat!B21*COS(RADIANS(26))</f>
-        <v>0.93725187499370022</v>
+        <f>18*Upper.dat!B21*COS(RADIANS(47))</f>
+        <v>0.71117987968785878</v>
       </c>
       <c r="C21">
-        <f>-Upper.dat!B21*SIN(RADIANS(26))+4</f>
-        <v>3.9746039842706176</v>
+        <f>-Upper.dat!B21*SIN(RADIANS(47))+4</f>
+        <v>3.9576307194346456</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1511,12 +1511,12 @@
         <v>52.251238200000003</v>
       </c>
       <c r="B22">
-        <f>18*Upper.dat!B22*COS(RADIANS(26))</f>
-        <v>0.94983587698638083</v>
+        <f>18*Upper.dat!B22*COS(RADIANS(47))</f>
+        <v>0.72072852852167035</v>
       </c>
       <c r="C22">
-        <f>-Upper.dat!B22*SIN(RADIANS(26))+4</f>
-        <v>3.9742630049447061</v>
+        <f>-Upper.dat!B22*SIN(RADIANS(47))+4</f>
+        <v>3.9570618487550684</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1525,12 +1525,12 @@
         <v>52.626149400000003</v>
       </c>
       <c r="B23">
-        <f>18*Upper.dat!B23*COS(RADIANS(26))</f>
-        <v>0.95859086071743516</v>
+        <f>18*Upper.dat!B23*COS(RADIANS(47))</f>
+        <v>0.72737174625496359</v>
       </c>
       <c r="C23">
-        <f>-Upper.dat!B23*SIN(RADIANS(26))+4</f>
-        <v>3.974025777673706</v>
+        <f>-Upper.dat!B23*SIN(RADIANS(47))+4</f>
+        <v>3.9566660721533427</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1539,12 +1539,12 @@
         <v>53.011275600000005</v>
       </c>
       <c r="B24">
-        <f>18*Upper.dat!B24*COS(RADIANS(26))</f>
-        <v>0.96356958741787058</v>
+        <f>18*Upper.dat!B24*COS(RADIANS(47))</f>
+        <v>0.7311495677246066</v>
       </c>
       <c r="C24">
-        <f>-Upper.dat!B24*SIN(RADIANS(26))+4</f>
-        <v>3.9738908728258524</v>
+        <f>-Upper.dat!B24*SIN(RADIANS(47))+4</f>
+        <v>3.9564410045124476</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1553,12 +1553,12 @@
         <v>53.4057186</v>
       </c>
       <c r="B25">
-        <f>18*Upper.dat!B25*COS(RADIANS(26))</f>
-        <v>0.96485396574583726</v>
+        <f>18*Upper.dat!B25*COS(RADIANS(47))</f>
+        <v>0.73212414462237296</v>
       </c>
       <c r="C25">
-        <f>-Upper.dat!B25*SIN(RADIANS(26))+4</f>
-        <v>3.9738560709832638</v>
+        <f>-Upper.dat!B25*SIN(RADIANS(47))+4</f>
+        <v>3.9563829430807433</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1567,12 +1567,12 @@
         <v>53.808556800000005</v>
       </c>
       <c r="B26">
-        <f>18*Upper.dat!B26*COS(RADIANS(26))</f>
-        <v>0.962546962640213</v>
+        <f>18*Upper.dat!B26*COS(RADIANS(47))</f>
+        <v>0.73037360750970148</v>
       </c>
       <c r="C26">
-        <f>-Upper.dat!B26*SIN(RADIANS(26))+4</f>
-        <v>3.9739185821275158</v>
+        <f>-Upper.dat!B26*SIN(RADIANS(47))+4</f>
+        <v>3.9564872331488194</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1581,12 +1581,12 @@
         <v>54.218846999999997</v>
       </c>
       <c r="B27">
-        <f>18*Upper.dat!B27*COS(RADIANS(26))</f>
-        <v>0.95677421911142047</v>
+        <f>18*Upper.dat!B27*COS(RADIANS(47))</f>
+        <v>0.72599329186797157</v>
       </c>
       <c r="C27">
-        <f>-Upper.dat!B27*SIN(RADIANS(26))+4</f>
-        <v>3.9740750018577615</v>
+        <f>-Upper.dat!B27*SIN(RADIANS(47))+4</f>
+        <v>3.9567481950062762</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1595,12 +1595,12 @@
         <v>54.635633400000003</v>
       </c>
       <c r="B28">
-        <f>18*Upper.dat!B28*COS(RADIANS(26))</f>
-        <v>0.94768242221982102</v>
+        <f>18*Upper.dat!B28*COS(RADIANS(47))</f>
+        <v>0.7190945027675949</v>
       </c>
       <c r="C28">
-        <f>-Upper.dat!B28*SIN(RADIANS(26))+4</f>
-        <v>3.9743213555040202</v>
+        <f>-Upper.dat!B28*SIN(RADIANS(47))+4</f>
+        <v>3.9571591975378486</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1609,12 +1609,12 @@
         <v>55.057942199999999</v>
       </c>
       <c r="B29">
-        <f>18*Upper.dat!B29*COS(RADIANS(26))</f>
-        <v>0.9354360755325406</v>
+        <f>18*Upper.dat!B29*COS(RADIANS(47))</f>
+        <v>0.7098020643142342</v>
       </c>
       <c r="C29">
-        <f>-Upper.dat!B29*SIN(RADIANS(26))+4</f>
-        <v>3.9746531856357015</v>
+        <f>-Upper.dat!B29*SIN(RADIANS(47))+4</f>
+        <v>3.9577128042176937</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1623,12 +1623,12 @@
         <v>55.484786999999997</v>
       </c>
       <c r="B30">
-        <f>18*Upper.dat!B30*COS(RADIANS(26))</f>
-        <v>0.9202110216909436</v>
+        <f>18*Upper.dat!B30*COS(RADIANS(47))</f>
+        <v>0.6982494046202955</v>
       </c>
       <c r="C30">
-        <f>-Upper.dat!B30*SIN(RADIANS(26))+4</f>
-        <v>3.9750657275757688</v>
+        <f>-Upper.dat!B30*SIN(RADIANS(47))+4</f>
+        <v>3.9584010659273239</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1637,12 +1637,12 @@
         <v>55.915170599999996</v>
       </c>
       <c r="B31">
-        <f>18*Upper.dat!B31*COS(RADIANS(26))</f>
-        <v>0.90219767603073353</v>
+        <f>18*Upper.dat!B31*COS(RADIANS(47))</f>
+        <v>0.68458100945225164</v>
       </c>
       <c r="C31">
-        <f>-Upper.dat!B31*SIN(RADIANS(26))+4</f>
-        <v>3.9755538217817459</v>
+        <f>-Upper.dat!B31*SIN(RADIANS(47))+4</f>
+        <v>3.9592153747770165</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1651,12 +1651,12 @@
         <v>56.348086800000004</v>
       </c>
       <c r="B32">
-        <f>18*Upper.dat!B32*COS(RADIANS(26))</f>
-        <v>0.88159617105563848</v>
+        <f>18*Upper.dat!B32*COS(RADIANS(47))</f>
+        <v>0.66894873789272513</v>
       </c>
       <c r="C32">
-        <f>-Upper.dat!B32*SIN(RADIANS(26))+4</f>
-        <v>3.9761120454122936</v>
+        <f>-Upper.dat!B32*SIN(RADIANS(47))+4</f>
+        <v>3.9601466836040742</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1665,12 +1665,12 @@
         <v>56.782525800000002</v>
       </c>
       <c r="B33">
-        <f>18*Upper.dat!B33*COS(RADIANS(26))</f>
-        <v>0.85861149683416638</v>
+        <f>18*Upper.dat!B33*COS(RADIANS(47))</f>
+        <v>0.6515081349090277</v>
       </c>
       <c r="C33">
-        <f>-Upper.dat!B33*SIN(RADIANS(26))+4</f>
-        <v>3.9767348440042589</v>
+        <f>-Upper.dat!B33*SIN(RADIANS(47))+4</f>
+        <v>3.96118572565539</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1679,12 +1679,12 @@
         <v>57.217474199999998</v>
       </c>
       <c r="B34">
-        <f>18*Upper.dat!B34*COS(RADIANS(26))</f>
-        <v>0.83345350099960469</v>
+        <f>18*Upper.dat!B34*COS(RADIANS(47))</f>
+        <v>0.63241843135315967</v>
       </c>
       <c r="C34">
-        <f>-Upper.dat!B34*SIN(RADIANS(26))+4</f>
-        <v>3.9774165314726768</v>
+        <f>-Upper.dat!B34*SIN(RADIANS(47))+4</f>
+        <v>3.9623230145874433</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1693,12 +1693,12 @@
         <v>57.651913199999996</v>
       </c>
       <c r="B35">
-        <f>18*Upper.dat!B35*COS(RADIANS(26))</f>
-        <v>0.80633365512991939</v>
+        <f>18*Upper.dat!B35*COS(RADIANS(47))</f>
+        <v>0.61184009031448661</v>
       </c>
       <c r="C35">
-        <f>-Upper.dat!B35*SIN(RADIANS(26))+4</f>
-        <v>3.9781513777297617</v>
+        <f>-Upper.dat!B35*SIN(RADIANS(47))+4</f>
+        <v>3.9635489906448926</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1707,12 +1707,12 @@
         <v>58.084829400000004</v>
       </c>
       <c r="B36">
-        <f>18*Upper.dat!B36*COS(RADIANS(26))</f>
-        <v>0.77746342468768126</v>
+        <f>18*Upper.dat!B36*COS(RADIANS(47))</f>
+        <v>0.58993357024205717</v>
       </c>
       <c r="C36">
-        <f>-Upper.dat!B36*SIN(RADIANS(26))+4</f>
-        <v>3.9789336528534331</v>
+        <f>-Upper.dat!B36*SIN(RADIANS(47))+4</f>
+        <v>3.9648540943488482</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1721,12 +1721,12 @@
         <v>58.515214799999995</v>
       </c>
       <c r="B37">
-        <f>18*Upper.dat!B37*COS(RADIANS(26))</f>
-        <v>0.74705426902006666</v>
+        <f>18*Upper.dat!B37*COS(RADIANS(47))</f>
+        <v>0.56685932494460289</v>
       </c>
       <c r="C37">
-        <f>-Upper.dat!B37*SIN(RADIANS(26))+4</f>
-        <v>3.9797576270873147</v>
+        <f>-Upper.dat!B37*SIN(RADIANS(47))+4</f>
+        <v>3.9662287664968718</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1735,12 +1735,12 @@
         <v>58.942057800000001</v>
       </c>
       <c r="B38">
-        <f>18*Upper.dat!B38*COS(RADIANS(26))</f>
-        <v>0.71531118023404849</v>
+        <f>18*Upper.dat!B38*COS(RADIANS(47))</f>
+        <v>0.542772900936208</v>
       </c>
       <c r="C38">
-        <f>-Upper.dat!B38*SIN(RADIANS(26))+4</f>
-        <v>3.9806177459130194</v>
+        <f>-Upper.dat!B38*SIN(RADIANS(47))+4</f>
+        <v>3.9676637402437045</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1749,12 +1749,12 @@
         <v>59.364366599999997</v>
       </c>
       <c r="B39">
-        <f>18*Upper.dat!B39*COS(RADIANS(26))</f>
-        <v>0.6824375101842024</v>
+        <f>18*Upper.dat!B39*COS(RADIANS(47))</f>
+        <v>0.51782860011941312</v>
       </c>
       <c r="C39">
-        <f>-Upper.dat!B39*SIN(RADIANS(26))+4</f>
-        <v>3.9815084992568566</v>
+        <f>-Upper.dat!B39*SIN(RADIANS(47))+4</f>
+        <v>3.9691498228931144</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1763,12 +1763,12 @@
         <v>59.781153000000003</v>
       </c>
       <c r="B40">
-        <f>18*Upper.dat!B40*COS(RADIANS(26))</f>
-        <v>0.64863175316032384</v>
+        <f>18*Upper.dat!B40*COS(RADIANS(47))</f>
+        <v>0.49217703851206984</v>
       </c>
       <c r="C40">
-        <f>-Upper.dat!B40*SIN(RADIANS(26))+4</f>
-        <v>3.9824245086669503</v>
+        <f>-Upper.dat!B40*SIN(RADIANS(47))+4</f>
+        <v>3.9706780413392804</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1777,12 +1777,12 @@
         <v>60.191445000000002</v>
       </c>
       <c r="B41">
-        <f>18*Upper.dat!B41*COS(RADIANS(26))</f>
-        <v>0.61408753161817464</v>
+        <f>18*Upper.dat!B41*COS(RADIANS(47))</f>
+        <v>0.46596513541993506</v>
       </c>
       <c r="C41">
-        <f>-Upper.dat!B41*SIN(RADIANS(26))+4</f>
-        <v>3.9833605276998805</v>
+        <f>-Upper.dat!B41*SIN(RADIANS(47))+4</f>
+        <v>3.9722396427118469</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1791,12 +1791,12 @@
         <v>60.5942814</v>
       </c>
       <c r="B42">
-        <f>18*Upper.dat!B42*COS(RADIANS(26))</f>
-        <v>0.57899522012416038</v>
+        <f>18*Upper.dat!B42*COS(RADIANS(47))</f>
+        <v>0.43933734567403604</v>
       </c>
       <c r="C42">
-        <f>-Upper.dat!B42*SIN(RADIANS(26))+4</f>
-        <v>3.9843113979178657</v>
+        <f>-Upper.dat!B42*SIN(RADIANS(47))+4</f>
+        <v>3.9738260209641036</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1805,12 +1805,12 @@
         <v>60.988724399999995</v>
       </c>
       <c r="B43">
-        <f>18*Upper.dat!B43*COS(RADIANS(26))</f>
-        <v>0.54353545976894313</v>
+        <f>18*Upper.dat!B43*COS(RADIANS(47))</f>
+        <v>0.41243073841507139</v>
       </c>
       <c r="C43">
-        <f>-Upper.dat!B43*SIN(RADIANS(26))+4</f>
-        <v>3.9852722246238641</v>
+        <f>-Upper.dat!B43*SIN(RADIANS(47))+4</f>
+        <v>3.9754290100595169</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1819,12 +1819,12 @@
         <v>61.373850599999997</v>
       </c>
       <c r="B44">
-        <f>18*Upper.dat!B44*COS(RADIANS(26))</f>
-        <v>0.50788887533546534</v>
+        <f>18*Upper.dat!B44*COS(RADIANS(47))</f>
+        <v>0.38538237040956141</v>
       </c>
       <c r="C44">
-        <f>-Upper.dat!B44*SIN(RADIANS(26))+4</f>
-        <v>3.9862381135627127</v>
+        <f>-Upper.dat!B44*SIN(RADIANS(47))+4</f>
+        <v>3.9770404446987579</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1833,12 +1833,12 @@
         <v>61.748763600000004</v>
       </c>
       <c r="B45">
-        <f>18*Upper.dat!B45*COS(RADIANS(26))</f>
-        <v>0.47222958971256318</v>
+        <f>18*Upper.dat!B45*COS(RADIANS(47))</f>
+        <v>0.35832436483425006</v>
       </c>
       <c r="C45">
-        <f>-Upper.dat!B45*SIN(RADIANS(26))+4</f>
-        <v>3.9872043466562275</v>
+        <f>-Upper.dat!B45*SIN(RADIANS(47))+4</f>
+        <v>3.9786524535062378</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1847,12 +1847,12 @@
         <v>62.112583200000003</v>
       </c>
       <c r="B46">
-        <f>18*Upper.dat!B46*COS(RADIANS(26))</f>
-        <v>0.43673170744288825</v>
+        <f>18*Upper.dat!B46*COS(RADIANS(47))</f>
+        <v>0.33138883094493043</v>
       </c>
       <c r="C46">
-        <f>-Upper.dat!B46*SIN(RADIANS(26))+4</f>
-        <v>3.9881662063233385</v>
+        <f>-Upper.dat!B46*SIN(RADIANS(47))+4</f>
+        <v>3.980257165935722</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1861,12 +1861,12 @@
         <v>62.4644634</v>
       </c>
       <c r="B47">
-        <f>18*Upper.dat!B47*COS(RADIANS(26))</f>
-        <v>0.40156444085040965</v>
+        <f>18*Upper.dat!B47*COS(RADIANS(47))</f>
+        <v>0.30470416581757831</v>
       </c>
       <c r="C47">
-        <f>-Upper.dat!B47*SIN(RADIANS(26))+4</f>
-        <v>3.9891191075437793</v>
+        <f>-Upper.dat!B47*SIN(RADIANS(47))+4</f>
+        <v>3.9818469325979478</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1875,12 +1875,12 @@
         <v>62.803579799999994</v>
       </c>
       <c r="B48">
-        <f>18*Upper.dat!B48*COS(RADIANS(26))</f>
-        <v>0.3668905064803839</v>
+        <f>18*Upper.dat!B48*COS(RADIANS(47))</f>
+        <v>0.27839383757870939</v>
       </c>
       <c r="C48">
-        <f>-Upper.dat!B48*SIN(RADIANS(26))+4</f>
-        <v>3.9900586413085599</v>
+        <f>-Upper.dat!B48*SIN(RADIANS(47))+4</f>
+        <v>3.9834143977509386</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1889,12 +1889,12 @@
         <v>63.129142200000004</v>
       </c>
       <c r="B49">
-        <f>18*Upper.dat!B49*COS(RADIANS(26))</f>
-        <v>0.33287905346436802</v>
+        <f>18*Upper.dat!B49*COS(RADIANS(47))</f>
+        <v>0.2525861953543585</v>
       </c>
       <c r="C49">
-        <f>-Upper.dat!B49*SIN(RADIANS(26))+4</f>
-        <v>3.9909802243096926</v>
+        <f>-Upper.dat!B49*SIN(RADIANS(47))+4</f>
+        <v>3.9849519148621004</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1903,12 +1903,12 @@
         <v>63.440391000000005</v>
       </c>
       <c r="B50">
-        <f>18*Upper.dat!B50*COS(RADIANS(26))</f>
-        <v>0.29969110713359903</v>
+        <f>18*Upper.dat!B50*COS(RADIANS(47))</f>
+        <v>0.22740342399019128</v>
       </c>
       <c r="C50">
-        <f>-Upper.dat!B50*SIN(RADIANS(26))+4</f>
-        <v>3.9918794933637534</v>
+        <f>-Upper.dat!B50*SIN(RADIANS(47))+4</f>
+        <v>3.986452204642247</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1917,12 +1917,12 @@
         <v>63.736597200000006</v>
       </c>
       <c r="B51">
-        <f>18*Upper.dat!B51*COS(RADIANS(26))</f>
-        <v>0.26748765816541076</v>
+        <f>18*Upper.dat!B51*COS(RADIANS(47))</f>
+        <v>0.20296768203674448</v>
       </c>
       <c r="C51">
-        <f>-Upper.dat!B51*SIN(RADIANS(26))+4</f>
-        <v>3.9927520862263091</v>
+        <f>-Upper.dat!B51*SIN(RADIANS(47))+4</f>
+        <v>3.987907989368753</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1931,12 +1931,12 @@
         <v>64.017069599999999</v>
       </c>
       <c r="B52">
-        <f>18*Upper.dat!B52*COS(RADIANS(26))</f>
-        <v>0.23642803660009076</v>
+        <f>18*Upper.dat!B52*COS(RADIANS(47))</f>
+        <v>0.17939986796528884</v>
       </c>
       <c r="C52">
-        <f>-Upper.dat!B52*SIN(RADIANS(26))+4</f>
-        <v>3.9935936856499721</v>
+        <f>-Upper.dat!B52*SIN(RADIANS(47))+4</f>
+        <v>3.9893120663895258</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1945,12 +1945,12 @@
         <v>64.281153000000003</v>
       </c>
       <c r="B53">
-        <f>18*Upper.dat!B53*COS(RADIANS(26))</f>
-        <v>0.20667153170862884</v>
+        <f>18*Upper.dat!B53*COS(RADIANS(47))</f>
+        <v>0.15682084931164963</v>
       </c>
       <c r="C53">
-        <f>-Upper.dat!B53*SIN(RADIANS(26))+4</f>
-        <v>3.9943999754920489</v>
+        <f>-Upper.dat!B53*SIN(RADIANS(47))+4</f>
+        <v>3.9906572348954827</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1959,12 +1959,12 @@
         <v>64.5282318</v>
       </c>
       <c r="B54">
-        <f>18*Upper.dat!B54*COS(RADIANS(26))</f>
-        <v>0.17837091659865353</v>
+        <f>18*Upper.dat!B54*COS(RADIANS(47))</f>
+        <v>0.1353465491944694</v>
       </c>
       <c r="C54">
-        <f>-Upper.dat!B54*SIN(RADIANS(26))+4</f>
-        <v>3.9951668161734708</v>
+        <f>-Upper.dat!B54*SIN(RADIANS(47))+4</f>
+        <v>3.9919365886463352</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1973,12 +1973,12 @@
         <v>64.757728200000003</v>
       </c>
       <c r="B55">
-        <f>18*Upper.dat!B55*COS(RADIANS(26))</f>
-        <v>0.15167892157003057</v>
+        <f>18*Upper.dat!B55*COS(RADIANS(47))</f>
+        <v>0.11509285825017268</v>
       </c>
       <c r="C55">
-        <f>-Upper.dat!B55*SIN(RADIANS(26))+4</f>
-        <v>3.9958900692750983</v>
+        <f>-Upper.dat!B55*SIN(RADIANS(47))+4</f>
+        <v>3.9931432233369559</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1987,12 +1987,12 @@
         <v>64.969104000000002</v>
       </c>
       <c r="B56">
-        <f>18*Upper.dat!B56*COS(RADIANS(26))</f>
-        <v>0.126738525100698</v>
+        <f>18*Upper.dat!B56*COS(RADIANS(47))</f>
+        <v>9.6168267503905405E-2</v>
       </c>
       <c r="C56">
-        <f>-Upper.dat!B56*SIN(RADIANS(26))+4</f>
-        <v>3.9965658606156453</v>
+        <f>-Upper.dat!B56*SIN(RADIANS(47))+4</f>
+        <v>3.9942706755017516</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2001,12 +2001,12 @@
         <v>65.161869600000003</v>
       </c>
       <c r="B57">
-        <f>18*Upper.dat!B57*COS(RADIANS(26))</f>
-        <v>0.10369426845932486</v>
+        <f>18*Upper.dat!B57*COS(RADIANS(47))</f>
+        <v>7.8682453815009823E-2</v>
       </c>
       <c r="C57">
-        <f>-Upper.dat!B57*SIN(RADIANS(26))+4</f>
-        <v>3.9971902736680494</v>
+        <f>-Upper.dat!B57*SIN(RADIANS(47))+4</f>
+        <v>3.9953124110278235</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2015,12 +2015,12 @@
         <v>65.335571399999992</v>
       </c>
       <c r="B58">
-        <f>18*Upper.dat!B58*COS(RADIANS(26))</f>
-        <v>8.2676091681732317E-2</v>
+        <f>18*Upper.dat!B58*COS(RADIANS(47))</f>
+        <v>6.2734014733949697E-2</v>
       </c>
       <c r="C58">
-        <f>-Upper.dat!B58*SIN(RADIANS(26))+4</f>
-        <v>3.9977597875439757</v>
+        <f>-Upper.dat!B58*SIN(RADIANS(47))+4</f>
+        <v>3.9962625558636158</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2029,12 +2029,12 @@
         <v>65.489806200000004</v>
       </c>
       <c r="B59">
-        <f>18*Upper.dat!B59*COS(RADIANS(26))</f>
-        <v>6.381064206815773E-2</v>
+        <f>18*Upper.dat!B59*COS(RADIANS(47))</f>
+        <v>4.8419049307468667E-2</v>
       </c>
       <c r="C59">
-        <f>-Upper.dat!B59*SIN(RADIANS(26))+4</f>
-        <v>3.9982709705758914</v>
+        <f>-Upper.dat!B59*SIN(RADIANS(47))+4</f>
+        <v>3.9971153848085295</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2043,12 +2043,12 @@
         <v>65.624212200000002</v>
       </c>
       <c r="B60">
-        <f>18*Upper.dat!B60*COS(RADIANS(26))</f>
-        <v>4.7211577399879044E-2</v>
+        <f>18*Upper.dat!B60*COS(RADIANS(47))</f>
+        <v>3.5823800230162989E-2</v>
       </c>
       <c r="C60">
-        <f>-Upper.dat!B60*SIN(RADIANS(26))+4</f>
-        <v>3.9987207430635823</v>
+        <f>-Upper.dat!B60*SIN(RADIANS(47))+4</f>
+        <v>3.9978657598643887</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2057,12 +2057,12 @@
         <v>65.738476200000008</v>
       </c>
       <c r="B61">
-        <f>18*Upper.dat!B61*COS(RADIANS(26))</f>
-        <v>3.2982793443922041E-2</v>
+        <f>18*Upper.dat!B61*COS(RADIANS(47))</f>
+        <v>2.5027102851488712E-2</v>
       </c>
       <c r="C61">
-        <f>-Upper.dat!B61*SIN(RADIANS(26))+4</f>
-        <v>3.9991062898208591</v>
+        <f>-Upper.dat!B61*SIN(RADIANS(47))+4</f>
+        <v>3.9985089843333053</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2071,12 +2071,12 @@
         <v>65.832329999999999</v>
       </c>
       <c r="B62">
-        <f>18*Upper.dat!B62*COS(RADIANS(26))</f>
-        <v>2.1213574542139974E-2</v>
+        <f>18*Upper.dat!B62*COS(RADIANS(47))</f>
+        <v>1.6096705478161819E-2</v>
       </c>
       <c r="C62">
-        <f>-Upper.dat!B62*SIN(RADIANS(26))+4</f>
-        <v>3.9994251915764347</v>
+        <f>-Upper.dat!B62*SIN(RADIANS(47))+4</f>
+        <v>3.9990410220394854</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2085,12 +2085,12 @@
         <v>65.905557600000009</v>
       </c>
       <c r="B63">
-        <f>18*Upper.dat!B63*COS(RADIANS(26))</f>
-        <v>1.1978585457354056E-2</v>
+        <f>18*Upper.dat!B63*COS(RADIANS(47))</f>
+        <v>9.0892631870691659E-3</v>
       </c>
       <c r="C63">
-        <f>-Upper.dat!B63*SIN(RADIANS(26))+4</f>
-        <v>3.9996754251948627</v>
+        <f>-Upper.dat!B63*SIN(RADIANS(47))+4</f>
+        <v>3.9994584976978338</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2099,12 +2099,12 @@
         <v>65.957984400000001</v>
       </c>
       <c r="B64">
-        <f>18*Upper.dat!B64*COS(RADIANS(26))</f>
-        <v>5.3378836041428216E-3</v>
+        <f>18*Upper.dat!B64*COS(RADIANS(47))</f>
+        <v>4.0503471059021379E-3</v>
       </c>
       <c r="C64">
-        <f>-Upper.dat!B64*SIN(RADIANS(26))+4</f>
-        <v>3.999855363345127</v>
+        <f>-Upper.dat!B64*SIN(RADIANS(47))+4</f>
+        <v>3.9997586963610496</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2113,12 +2113,12 @@
         <v>65.989489800000001</v>
       </c>
       <c r="B65">
-        <f>18*Upper.dat!B65*COS(RADIANS(26))</f>
-        <v>1.3369047795878518E-3</v>
+        <f>18*Upper.dat!B65*COS(RADIANS(47))</f>
+        <v>1.0144335857506846E-3</v>
       </c>
       <c r="C65">
-        <f>-Upper.dat!B65*SIN(RADIANS(26))+4</f>
-        <v>3.9999637748872883</v>
+        <f>-Upper.dat!B65*SIN(RADIANS(47))+4</f>
+        <v>3.9999395640646802</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2127,11 +2127,11 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <f>18*Upper.dat!B66*COS(RADIANS(26))</f>
+        <f>18*Upper.dat!B66*COS(RADIANS(47))</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f>-Upper.dat!B66*SIN(RADIANS(26))+4</f>
+        <f>-Upper.dat!B66*SIN(RADIANS(47))+4</f>
         <v>4</v>
       </c>
     </row>
@@ -2146,7 +2146,7 @@
   <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C66"/>
+      <selection activeCell="C1" sqref="C1:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2157,12 +2157,12 @@
         <v>51</v>
       </c>
       <c r="B1">
-        <f>12*Upper.dat!B1*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4523094954143154</v>
+        <f>12*Upper.dat!B1*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.940611048575114</v>
       </c>
       <c r="C1">
-        <f>4-12*Upper.dat!B1*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.279498787085842</v>
+        <f>4-12*Upper.dat!B1*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.459950801874953</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2171,12 +2171,12 @@
         <v>51.007006799999999</v>
       </c>
       <c r="B2">
-        <f>12*Upper.dat!B2*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4982511476553402</v>
+        <f>12*Upper.dat!B2*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.975471238866707</v>
       </c>
       <c r="C2">
-        <f>4-12*Upper.dat!B2*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.257091546115333</v>
+        <f>4-12*Upper.dat!B2*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.422567824580742</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2185,12 +2185,12 @@
         <v>51.028010399999999</v>
       </c>
       <c r="B3">
-        <f>12*Upper.dat!B3*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5431879158247774</v>
+        <f>12*Upper.dat!B3*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.009568930461633</v>
       </c>
       <c r="C3">
-        <f>4-12*Upper.dat!B3*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.235174419854268</v>
+        <f>4-12*Upper.dat!B3*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.386002527030271</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2199,12 +2199,12 @@
         <v>51.062961599999994</v>
       </c>
       <c r="B4">
-        <f>12*Upper.dat!B4*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5870691636564578</v>
+        <f>12*Upper.dat!B4*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.042865700930829</v>
       </c>
       <c r="C4">
-        <f>4-12*Upper.dat!B4*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.213772105259824</v>
+        <f>4-12*Upper.dat!B4*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.350296112234233</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2213,12 +2213,12 @@
         <v>51.111778799999996</v>
       </c>
       <c r="B5">
-        <f>12*Upper.dat!B5*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.629827034730889</v>
+        <f>12*Upper.dat!B5*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.075310061318614</v>
       </c>
       <c r="C5">
-        <f>4-12*Upper.dat!B5*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.192917698119125</v>
+        <f>4-12*Upper.dat!B5*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.315503795337609</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2227,12 +2227,12 @@
         <v>51.174349199999995</v>
       </c>
       <c r="B6">
-        <f>12*Upper.dat!B6*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.6713818438805594</v>
+        <f>12*Upper.dat!B6*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.106841547101681</v>
       </c>
       <c r="C6">
-        <f>4-12*Upper.dat!B6*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.172650063485197</v>
+        <f>4-12*Upper.dat!B6*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.281690416603261</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2241,12 +2241,12 @@
         <v>51.250525199999998</v>
       </c>
       <c r="B7">
-        <f>12*Upper.dat!B7*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7116399241611582</v>
+        <f>12*Upper.dat!B7*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.137389084486561</v>
       </c>
       <c r="C7">
-        <f>4-12*Upper.dat!B7*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.15301488577925</v>
+        <f>4-12*Upper.dat!B7*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.248932193343407</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2255,12 +2255,12 @@
         <v>51.340129200000007</v>
       </c>
       <c r="B8">
-        <f>12*Upper.dat!B8*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7504968570742321</v>
+        <f>12*Upper.dat!B8*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.166873441479012</v>
       </c>
       <c r="C8">
-        <f>4-12*Upper.dat!B8*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.134063093305826</v>
+        <f>4-12*Upper.dat!B8*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.217314091469504</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2269,12 +2269,12 @@
         <v>51.442952399999996</v>
       </c>
       <c r="B9">
-        <f>12*Upper.dat!B9*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7878407095847306</v>
+        <f>12*Upper.dat!B9*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.195209684109283</v>
       </c>
       <c r="C9">
-        <f>4-12*Upper.dat!B9*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.115849279453858</v>
+        <f>4-12*Upper.dat!B9*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.186927191513131</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2283,12 +2283,12 @@
         <v>51.558753600000003</v>
       </c>
       <c r="B10">
-        <f>12*Upper.dat!B10*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8235531140328387</v>
+        <f>12*Upper.dat!B10*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.222307995861328</v>
       </c>
       <c r="C10">
-        <f>4-12*Upper.dat!B10*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.09843117598847</v>
+        <f>4-12*Upper.dat!B10*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.157867809895745</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2297,12 +2297,12 @@
         <v>51.687263999999999</v>
       </c>
       <c r="B11">
-        <f>12*Upper.dat!B11*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8575135769094917</v>
+        <f>12*Upper.dat!B11*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.24807694714022</v>
       </c>
       <c r="C11">
-        <f>4-12*Upper.dat!B11*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.081867551520745</v>
+        <f>4-12*Upper.dat!B11*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.130233992854109</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2311,12 +2311,12 @@
         <v>51.828182400000003</v>
       </c>
       <c r="B12">
-        <f>12*Upper.dat!B12*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8895984057394273</v>
+        <f>12*Upper.dat!B12*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.272422680998829</v>
       </c>
       <c r="C12">
-        <f>4-12*Upper.dat!B12*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.066218734901828</v>
+        <f>4-12*Upper.dat!B12*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.10412638964155</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2325,12 +2325,12 @@
         <v>51.981178799999995</v>
       </c>
       <c r="B13">
-        <f>12*Upper.dat!B13*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9196904119799525</v>
+        <f>12*Upper.dat!B13*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.295256275626578</v>
       </c>
       <c r="C13">
-        <f>4-12*Upper.dat!B13*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.051541882802997</v>
+        <f>4-12*Upper.dat!B13*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.079640357225365</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2339,12 +2339,12 @@
         <v>52.145898000000003</v>
       </c>
       <c r="B14">
-        <f>12*Upper.dat!B14*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9476735141797406</v>
+        <f>12*Upper.dat!B14*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.31648964926573</v>
       </c>
       <c r="C14">
-        <f>4-12*Upper.dat!B14*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.03789361193099</v>
+        <f>4-12*Upper.dat!B14*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.056870351726474</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2353,12 +2353,12 @@
         <v>52.321953600000001</v>
       </c>
       <c r="B15">
-        <f>12*Upper.dat!B15*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9734435303022675</v>
+        <f>12*Upper.dat!B15*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.336043749347628</v>
       </c>
       <c r="C15">
-        <f>4-12*Upper.dat!B15*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.025324735260167</v>
+        <f>4-12*Upper.dat!B15*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.035901146645955</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2367,12 +2367,12 @@
         <v>52.508935199999996</v>
       </c>
       <c r="B16">
-        <f>12*Upper.dat!B16*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9969016982548169</v>
+        <f>12*Upper.dat!B16*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.3538436359174</v>
       </c>
       <c r="C16">
-        <f>4-12*Upper.dat!B16*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.013883422281658</v>
+        <f>4-12*Upper.dat!B16*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.016813105246545</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2381,12 +2381,12 @@
         <v>52.706406000000001</v>
       </c>
       <c r="B17">
-        <f>12*Upper.dat!B17*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0179665426878497</v>
+        <f>12*Upper.dat!B17*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.369827486074676</v>
       </c>
       <c r="C17">
-        <f>4-12*Upper.dat!B17*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.003609411178598</v>
+        <f>4-12*Upper.dat!B17*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.999672524472157</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2395,12 +2395,12 @@
         <v>52.913905200000002</v>
       </c>
       <c r="B18">
-        <f>12*Upper.dat!B18*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0365674009599122</v>
+        <f>12*Upper.dat!B18*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.383941681523051</v>
       </c>
       <c r="C18">
-        <f>4-12*Upper.dat!B18*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.994537166424017</v>
+        <f>4-12*Upper.dat!B18*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.98453690290615</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2409,12 +2409,12 @@
         <v>53.130946800000004</v>
       </c>
       <c r="B19">
-        <f>12*Upper.dat!B19*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0526519743666025</v>
+        <f>12*Upper.dat!B19*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.396146538387462</v>
       </c>
       <c r="C19">
-        <f>4-12*Upper.dat!B19*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.986692195800394</v>
+        <f>4-12*Upper.dat!B19*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.971448796294421</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2423,12 +2423,12 @@
         <v>53.3570244</v>
       </c>
       <c r="B20">
-        <f>12*Upper.dat!B20*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0661841655989583</v>
+        <f>12*Upper.dat!B20*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.406414666293429</v>
       </c>
       <c r="C20">
-        <f>4-12*Upper.dat!B20*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.980092105141669</v>
+        <f>4-12*Upper.dat!B20*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.960437577217533</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2437,12 +2437,12 @@
         <v>53.591611200000003</v>
       </c>
       <c r="B21">
-        <f>12*Upper.dat!B21*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0771440787434496</v>
+        <f>12*Upper.dat!B21*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.414730968367021</v>
       </c>
       <c r="C21">
-        <f>4-12*Upper.dat!B21*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.974746598333251</v>
+        <f>4-12*Upper.dat!B21*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.951519435090702</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2451,12 +2451,12 @@
         <v>53.834158799999997</v>
       </c>
       <c r="B22">
-        <f>12*Upper.dat!B22*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0855334134052352</v>
+        <f>12*Upper.dat!B22*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.421096734256228</v>
       </c>
       <c r="C22">
-        <f>4-12*Upper.dat!B22*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.970654846422313</v>
+        <f>4-12*Upper.dat!B22*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.94469298693577</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2465,12 +2465,12 @@
         <v>54.084099600000002</v>
       </c>
       <c r="B23">
-        <f>12*Upper.dat!B23*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0913700692259383</v>
+        <f>12*Upper.dat!B23*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.425525546078422</v>
       </c>
       <c r="C23">
-        <f>4-12*Upper.dat!B23*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.967808119170314</v>
+        <f>4-12*Upper.dat!B23*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.939943667715063</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2479,12 +2479,12 @@
         <v>54.340850399999994</v>
       </c>
       <c r="B24">
-        <f>12*Upper.dat!B24*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0946892203595624</v>
+        <f>12*Upper.dat!B24*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.428044093724854</v>
       </c>
       <c r="C24">
-        <f>4-12*Upper.dat!B24*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.966189260996067</v>
+        <f>4-12*Upper.dat!B24*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.937242856024326</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2493,12 +2493,12 @@
         <v>54.603812399999995</v>
       </c>
       <c r="B25">
-        <f>12*Upper.dat!B25*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0955454725782072</v>
+        <f>12*Upper.dat!B25*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.428693811656697</v>
       </c>
       <c r="C25">
-        <f>4-12*Upper.dat!B25*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.965771638885006</v>
+        <f>4-12*Upper.dat!B25*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.936546118843875</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2507,12 +2507,12 @@
         <v>54.872371200000003</v>
       </c>
       <c r="B26">
-        <f>12*Upper.dat!B26*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0940074705077905</v>
+        <f>12*Upper.dat!B26*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.427526786914914</v>
       </c>
       <c r="C26">
-        <f>4-12*Upper.dat!B26*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.966521772616026</v>
+        <f>4-12*Upper.dat!B26*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.937797599660783</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2521,12 +2521,12 @@
         <v>55.145898000000003</v>
       </c>
       <c r="B27">
-        <f>12*Upper.dat!B27*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0901589748219287</v>
+        <f>12*Upper.dat!B27*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.424606576487097</v>
       </c>
       <c r="C27">
-        <f>4-12*Upper.dat!B27*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.968398809378979</v>
+        <f>4-12*Upper.dat!B27*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.940929141950267</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2535,12 +2535,12 @@
         <v>55.423755599999993</v>
       </c>
       <c r="B28">
-        <f>12*Upper.dat!B28*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0840977768941968</v>
+        <f>12*Upper.dat!B28*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.420007383753511</v>
       </c>
       <c r="C28">
-        <f>4-12*Upper.dat!B28*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.971355053134083</v>
+        <f>4-12*Upper.dat!B28*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.945861172329135</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2549,12 +2549,12 @@
         <v>55.705294800000004</v>
       </c>
       <c r="B29">
-        <f>12*Upper.dat!B29*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0759335457693417</v>
+        <f>12*Upper.dat!B29*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.413812424784602</v>
       </c>
       <c r="C29">
-        <f>4-12*Upper.dat!B29*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.975337014714256</v>
+        <f>4-12*Upper.dat!B29*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.952504452487279</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2563,12 +2563,12 @@
         <v>55.989857999999998</v>
       </c>
       <c r="B30">
-        <f>12*Upper.dat!B30*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0657835098749437</v>
+        <f>12*Upper.dat!B30*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.406110651655311</v>
       </c>
       <c r="C30">
-        <f>4-12*Upper.dat!B30*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.980287517995066</v>
+        <f>4-12*Upper.dat!B30*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.960763593002842</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2577,12 +2577,12 @@
         <v>56.276780400000007</v>
       </c>
       <c r="B31">
-        <f>12*Upper.dat!B31*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0537746127681373</v>
+        <f>12*Upper.dat!B31*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.396998388209948</v>
       </c>
       <c r="C31">
-        <f>4-12*Upper.dat!B31*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.986144648466791</v>
+        <f>4-12*Upper.dat!B31*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.970535299199149</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2591,12 +2591,12 @@
         <v>56.565391199999993</v>
       </c>
       <c r="B32">
-        <f>12*Upper.dat!B32*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0400402761180736</v>
+        <f>12*Upper.dat!B32*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.38657687383693</v>
       </c>
       <c r="C32">
-        <f>4-12*Upper.dat!B32*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>18.99284333203336</v>
+        <f>4-12*Upper.dat!B32*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.981711005123845</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2605,12 +2605,12 @@
         <v>56.855017200000006</v>
       </c>
       <c r="B33">
-        <f>12*Upper.dat!B33*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.024717159970427</v>
+        <f>12*Upper.dat!B33*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.374949805181132</v>
       </c>
       <c r="C33">
-        <f>4-12*Upper.dat!B33*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.000316915136949</v>
+        <f>4-12*Upper.dat!B33*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>23.994179509739631</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2619,12 +2619,12 @@
         <v>57.144982799999994</v>
       </c>
       <c r="B34">
-        <f>12*Upper.dat!B34*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>8.0079451627473848</v>
+        <f>12*Upper.dat!B34*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.362223336143888</v>
       </c>
       <c r="C34">
-        <f>4-12*Upper.dat!B34*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.008497164757962</v>
+        <f>4-12*Upper.dat!B34*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.007826976924271</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2633,12 +2633,12 @@
         <v>57.434608800000007</v>
       </c>
       <c r="B35">
-        <f>12*Upper.dat!B35*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9898652655009279</v>
+        <f>12*Upper.dat!B35*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.348504442118106</v>
       </c>
       <c r="C35">
-        <f>4-12*Upper.dat!B35*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.017315319842982</v>
+        <f>4-12*Upper.dat!B35*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.022538689613665</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2647,12 +2647,12 @@
         <v>57.723219599999993</v>
       </c>
       <c r="B36">
-        <f>12*Upper.dat!B36*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9706184452061031</v>
+        <f>12*Upper.dat!B36*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.333900095403152</v>
       </c>
       <c r="C36">
-        <f>4-12*Upper.dat!B36*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.02670262132704</v>
+        <f>4-12*Upper.dat!B36*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.038199934061133</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2661,12 +2661,12 @@
         <v>58.010143200000002</v>
       </c>
       <c r="B37">
-        <f>12*Upper.dat!B37*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9503456747610262</v>
+        <f>12*Upper.dat!B37*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.31851726520485</v>
       </c>
       <c r="C37">
-        <f>4-12*Upper.dat!B37*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.036590312133619</v>
+        <f>4-12*Upper.dat!B37*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.054695999837417</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2675,12 +2675,12 @@
         <v>58.294705199999996</v>
       </c>
       <c r="B38">
-        <f>12*Upper.dat!B38*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9291836155703477</v>
+        <f>12*Upper.dat!B38*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.302459649199253</v>
       </c>
       <c r="C38">
-        <f>4-12*Upper.dat!B38*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.04691173804207</v>
+        <f>4-12*Upper.dat!B38*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.071915684799407</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2689,12 +2689,12 @@
         <v>58.576244400000007</v>
       </c>
       <c r="B39">
-        <f>12*Upper.dat!B39*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.9072678355371169</v>
+        <f>12*Upper.dat!B39*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.285830115321389</v>
       </c>
       <c r="C39">
-        <f>4-12*Upper.dat!B39*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.057600778168119</v>
+        <f>4-12*Upper.dat!B39*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.089748676592325</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2703,12 +2703,12 @@
         <v>58.854101999999997</v>
       </c>
       <c r="B40">
-        <f>12*Upper.dat!B40*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8847306641878649</v>
+        <f>12*Upper.dat!B40*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.268729074249826</v>
       </c>
       <c r="C40">
-        <f>4-12*Upper.dat!B40*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.068592891089242</v>
+        <f>4-12*Upper.dat!B40*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.108087297946316</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2717,12 +2717,12 @@
         <v>59.127629999999996</v>
       </c>
       <c r="B41">
-        <f>12*Upper.dat!B41*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8617011831597647</v>
+        <f>12*Upper.dat!B41*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.251254472188403</v>
       </c>
       <c r="C41">
-        <f>4-12*Upper.dat!B41*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.079825119484404</v>
+        <f>4-12*Upper.dat!B41*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.126826514417118</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2731,12 +2731,12 @@
         <v>59.396187600000005</v>
       </c>
       <c r="B42">
-        <f>12*Upper.dat!B42*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8383063088304219</v>
+        <f>12*Upper.dat!B42*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.233502612357803</v>
       </c>
       <c r="C42">
-        <f>4-12*Upper.dat!B42*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.091235562100231</v>
+        <f>4-12*Upper.dat!B42*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.145863053444195</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2745,12 +2745,12 @@
         <v>59.659149600000006</v>
       </c>
       <c r="B43">
-        <f>12*Upper.dat!B43*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.8146664685936109</v>
+        <f>12*Upper.dat!B43*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.215564874185162</v>
       </c>
       <c r="C43">
-        <f>4-12*Upper.dat!B43*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.102765482572213</v>
+        <f>4-12*Upper.dat!B43*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.165098922589156</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2759,12 +2759,12 @@
         <v>59.915900399999998</v>
       </c>
       <c r="B44">
-        <f>12*Upper.dat!B44*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7909020789712926</v>
+        <f>12*Upper.dat!B44*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.197532628848155</v>
       </c>
       <c r="C44">
-        <f>4-12*Upper.dat!B44*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.114356149838393</v>
+        <f>4-12*Upper.dat!B44*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.18443613826005</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2773,12 +2773,12 @@
         <v>60.165842400000002</v>
       </c>
       <c r="B45">
-        <f>12*Upper.dat!B45*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7671292218893573</v>
+        <f>12*Upper.dat!B45*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.179493958464615</v>
       </c>
       <c r="C45">
-        <f>4-12*Upper.dat!B45*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.125950946960572</v>
+        <f>4-12*Upper.dat!B45*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.203780243949808</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2787,12 +2787,12 @@
         <v>60.408388799999997</v>
       </c>
       <c r="B46">
-        <f>12*Upper.dat!B46*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7434639670429073</v>
+        <f>12*Upper.dat!B46*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.161536935871734</v>
       </c>
       <c r="C46">
-        <f>4-12*Upper.dat!B46*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.137493262965901</v>
+        <f>4-12*Upper.dat!B46*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.223036793103617</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2801,12 +2801,12 @@
         <v>60.6429756</v>
       </c>
       <c r="B47">
-        <f>12*Upper.dat!B47*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.7200191226479218</v>
+        <f>12*Upper.dat!B47*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.143747159120167</v>
       </c>
       <c r="C47">
-        <f>4-12*Upper.dat!B47*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.148928077611192</v>
+        <f>4-12*Upper.dat!B47*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.242113993050324</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2815,12 +2815,12 @@
         <v>60.869053199999996</v>
       </c>
       <c r="B48">
-        <f>12*Upper.dat!B48*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.6969031664012384</v>
+        <f>12*Upper.dat!B48*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.126206940294253</v>
       </c>
       <c r="C48">
-        <f>4-12*Upper.dat!B48*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.160202482788563</v>
+        <f>4-12*Upper.dat!B48*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.26092357488622</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2829,12 +2829,12 @@
         <v>61.086094799999998</v>
       </c>
       <c r="B49">
-        <f>12*Upper.dat!B49*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.6742288643905603</v>
+        <f>12*Upper.dat!B49*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.109001845478019</v>
       </c>
       <c r="C49">
-        <f>4-12*Upper.dat!B49*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.171261478802155</v>
+        <f>4-12*Upper.dat!B49*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.279373780220155</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2843,12 +2843,12 @@
         <v>61.293593999999999</v>
       </c>
       <c r="B50">
-        <f>12*Upper.dat!B50*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.6521035668367148</v>
+        <f>12*Upper.dat!B50*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.092213331235243</v>
       </c>
       <c r="C50">
-        <f>4-12*Upper.dat!B50*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.182052707450882</v>
+        <f>4-12*Upper.dat!B50*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.297377257581914</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2857,12 +2857,12 @@
         <v>61.491064800000004</v>
       </c>
       <c r="B51">
-        <f>12*Upper.dat!B51*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.6306346008579222</v>
+        <f>12*Upper.dat!B51*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.075922836599609</v>
       </c>
       <c r="C51">
-        <f>4-12*Upper.dat!B51*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.192523821801551</v>
+        <f>4-12*Upper.dat!B51*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.314846674299989</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2871,12 +2871,12 @@
         <v>61.678046399999999</v>
       </c>
       <c r="B52">
-        <f>12*Upper.dat!B52*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.6099281864810422</v>
+        <f>12*Upper.dat!B52*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.060210960551974</v>
       </c>
       <c r="C52">
-        <f>4-12*Upper.dat!B52*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.202623014885503</v>
+        <f>4-12*Upper.dat!B52*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.331695598549263</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2885,12 +2885,12 @@
         <v>61.854101999999997</v>
       </c>
       <c r="B53">
-        <f>12*Upper.dat!B53*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5900905165534009</v>
+        <f>12*Upper.dat!B53*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.045158281449549</v>
       </c>
       <c r="C53">
-        <f>4-12*Upper.dat!B53*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.212298492990428</v>
+        <f>4-12*Upper.dat!B53*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.347837620620748</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2899,12 +2899,12 @@
         <v>62.018821200000005</v>
       </c>
       <c r="B54">
-        <f>12*Upper.dat!B54*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5712234398134175</v>
+        <f>12*Upper.dat!B54*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.030842081371429</v>
       </c>
       <c r="C54">
-        <f>4-12*Upper.dat!B54*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.22150058116749</v>
+        <f>4-12*Upper.dat!B54*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.363189865630975</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2913,12 +2913,12 @@
         <v>62.171818799999997</v>
       </c>
       <c r="B55">
-        <f>12*Upper.dat!B55*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5534287764610024</v>
+        <f>12*Upper.dat!B55*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.017339620741897</v>
       </c>
       <c r="C55">
-        <f>4-12*Upper.dat!B55*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.23017961838702</v>
+        <f>4-12*Upper.dat!B55*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.377669481918424</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2927,12 +2927,12 @@
         <v>62.312736000000001</v>
       </c>
       <c r="B56">
-        <f>12*Upper.dat!B56*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5368018454814472</v>
+        <f>12*Upper.dat!B56*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>22.00472322691105</v>
       </c>
       <c r="C56">
-        <f>4-12*Upper.dat!B56*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.238289114473584</v>
+        <f>4-12*Upper.dat!B56*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.391198907895973</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2941,12 +2941,12 @@
         <v>62.441246399999997</v>
       </c>
       <c r="B57">
-        <f>12*Upper.dat!B57*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5214390077205318</v>
+        <f>12*Upper.dat!B57*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.993066017785122</v>
       </c>
       <c r="C57">
-        <f>4-12*Upper.dat!B57*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.245782071102433</v>
+        <f>4-12*Upper.dat!B57*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.403699734208836</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2955,12 +2955,12 @@
         <v>62.557047600000004</v>
       </c>
       <c r="B58">
-        <f>12*Upper.dat!B58*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.5074268898688032</v>
+        <f>12*Upper.dat!B58*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.982433725064414</v>
       </c>
       <c r="C58">
-        <f>4-12*Upper.dat!B58*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.252616237613548</v>
+        <f>4-12*Upper.dat!B58*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.415101472238344</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2969,12 +2969,12 @@
         <v>62.659870799999993</v>
       </c>
       <c r="B59">
-        <f>12*Upper.dat!B59*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4948499234597543</v>
+        <f>12*Upper.dat!B59*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.972890414780093</v>
       </c>
       <c r="C59">
-        <f>4-12*Upper.dat!B59*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.258750433996539</v>
+        <f>4-12*Upper.dat!B59*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.425335419577305</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2983,12 +2983,12 @@
         <v>62.749474800000002</v>
       </c>
       <c r="B60">
-        <f>12*Upper.dat!B60*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.483783880347568</v>
+        <f>12*Upper.dat!B60*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.964493582061891</v>
       </c>
       <c r="C60">
-        <f>4-12*Upper.dat!B60*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.264147703848828</v>
+        <f>4-12*Upper.dat!B60*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.43433992024762</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2997,12 +2997,12 @@
         <v>62.825650800000005</v>
       </c>
       <c r="B61">
-        <f>12*Upper.dat!B61*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4742980243769299</v>
+        <f>12*Upper.dat!B61*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.957295783809439</v>
       </c>
       <c r="C61">
-        <f>4-12*Upper.dat!B61*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.268774264936148</v>
+        <f>4-12*Upper.dat!B61*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.442058613874615</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -3011,12 +3011,12 @@
         <v>62.888220000000004</v>
       </c>
       <c r="B62">
-        <f>12*Upper.dat!B62*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4664518784424088</v>
+        <f>12*Upper.dat!B62*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.951342185560556</v>
       </c>
       <c r="C62">
-        <f>4-12*Upper.dat!B62*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.272601086003057</v>
+        <f>4-12*Upper.dat!B62*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.448443066348776</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -3025,12 +3025,12 @@
         <v>62.937038400000006</v>
       </c>
       <c r="B63">
-        <f>12*Upper.dat!B63*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4602952190525516</v>
+        <f>12*Upper.dat!B63*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.946670557366495</v>
       </c>
       <c r="C63">
-        <f>4-12*Upper.dat!B63*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.275603889424193</v>
+        <f>4-12*Upper.dat!B63*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.453452774248959</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -3039,12 +3039,12 @@
         <v>62.971989600000001</v>
       </c>
       <c r="B64">
-        <f>12*Upper.dat!B64*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4558680844837442</v>
+        <f>12*Upper.dat!B64*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.943311279979049</v>
       </c>
       <c r="C64">
-        <f>4-12*Upper.dat!B64*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.277763147227365</v>
+        <f>4-12*Upper.dat!B64*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.457055158207549</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -3053,12 +3053,12 @@
         <v>62.992993200000001</v>
       </c>
       <c r="B65">
-        <f>12*Upper.dat!B65*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4532007652673737</v>
+        <f>12*Upper.dat!B65*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.941287337632282</v>
       </c>
       <c r="C65">
-        <f>4-12*Upper.dat!B65*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.279064085733296</v>
+        <f>4-12*Upper.dat!B65*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.459225570651114</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -3067,12 +3067,12 @@
         <v>63</v>
       </c>
       <c r="B66">
-        <f>12*Upper.dat!B66*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4523094954143154</v>
+        <f>12*Upper.dat!B66*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.940611048575114</v>
       </c>
       <c r="C66">
-        <f>4-12*Upper.dat!B66*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.279498787085842</v>
+        <f>4-12*Upper.dat!B66*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.459950801874953</v>
       </c>
     </row>
   </sheetData>
@@ -3905,11 +3905,11 @@
         <v>48</v>
       </c>
       <c r="B1">
-        <f>18*Lower.dat!B1*COS(RADIANS(26))</f>
+        <f>18*Lower.dat!B1*COS(RADIANS(47))</f>
         <v>0</v>
       </c>
       <c r="C1">
-        <f>-Lower.dat!B1*SIN(RADIANS(26))+4</f>
+        <f>-Lower.dat!B1*SIN(RADIANS(47))+4</f>
         <v>4</v>
       </c>
     </row>
@@ -3919,12 +3919,12 @@
         <v>48.010510199999999</v>
       </c>
       <c r="B2">
-        <f>18*Lower.dat!B2*COS(RADIANS(26))</f>
-        <v>-6.8912478361536522E-2</v>
+        <f>18*Lower.dat!B2*COS(RADIANS(47))</f>
+        <v>-5.2290285437390172E-2</v>
       </c>
       <c r="C2">
-        <f>-Lower.dat!B2*SIN(RADIANS(26))+4</f>
-        <v>4.0018672700808757</v>
+        <f>-Lower.dat!B2*SIN(RADIANS(47))+4</f>
+        <v>4.0031152481078509</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3933,12 +3933,12 @@
         <v>48.042015599999999</v>
       </c>
       <c r="B3">
-        <f>18*Lower.dat!B3*COS(RADIANS(26))</f>
-        <v>-0.13631763061569294</v>
+        <f>18*Lower.dat!B3*COS(RADIANS(47))</f>
+        <v>-0.10343682282977998</v>
       </c>
       <c r="C3">
-        <f>-Lower.dat!B3*SIN(RADIANS(26))+4</f>
-        <v>4.0036936972692976</v>
+        <f>-Lower.dat!B3*SIN(RADIANS(47))+4</f>
+        <v>4.0061623562370565</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3947,12 +3947,12 @@
         <v>48.094442400000005</v>
       </c>
       <c r="B4">
-        <f>18*Lower.dat!B4*COS(RADIANS(26))</f>
-        <v>-0.20213950236321315</v>
+        <f>18*Lower.dat!B4*COS(RADIANS(47))</f>
+        <v>-0.15338197853357172</v>
       </c>
       <c r="C4">
-        <f>-Lower.dat!B4*SIN(RADIANS(26))+4</f>
-        <v>4.0054772234855012</v>
+        <f>-Lower.dat!B4*SIN(RADIANS(47))+4</f>
+        <v>4.0091378908033937</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3961,12 +3961,12 @@
         <v>48.167668199999994</v>
       </c>
       <c r="B5">
-        <f>18*Lower.dat!B5*COS(RADIANS(26))</f>
-        <v>-0.26627630897485977</v>
+        <f>18*Lower.dat!B5*COS(RADIANS(47))</f>
+        <v>-0.20204851911524929</v>
       </c>
       <c r="C5">
-        <f>-Lower.dat!B5*SIN(RADIANS(26))+4</f>
-        <v>4.0072150907472261</v>
+        <f>-Lower.dat!B5*SIN(RADIANS(47))+4</f>
+        <v>4.012037250544779</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3975,12 +3975,12 @@
         <v>48.261523800000006</v>
       </c>
       <c r="B6">
-        <f>18*Lower.dat!B6*COS(RADIANS(26))</f>
-        <v>-0.32860852269936625</v>
+        <f>18*Lower.dat!B6*COS(RADIANS(47))</f>
+        <v>-0.24934574778984689</v>
       </c>
       <c r="C6">
-        <f>-Lower.dat!B6*SIN(RADIANS(26))+4</f>
-        <v>4.0089040603000532</v>
+        <f>-Lower.dat!B6*SIN(RADIANS(47))+4</f>
+        <v>4.0148550321059746</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3989,12 +3989,12 @@
         <v>48.375787799999998</v>
       </c>
       <c r="B7">
-        <f>18*Lower.dat!B7*COS(RADIANS(26))</f>
-        <v>-0.38899564312026419</v>
+        <f>18*Lower.dat!B7*COS(RADIANS(47))</f>
+        <v>-0.29516705386716907</v>
       </c>
       <c r="C7">
-        <f>-Lower.dat!B7*SIN(RADIANS(26))+4</f>
-        <v>4.0105403251088827</v>
+        <f>-Lower.dat!B7*SIN(RADIANS(47))+4</f>
+        <v>4.0175848840442958</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4003,12 +4003,12 @@
         <v>48.510193799999996</v>
       </c>
       <c r="B8">
-        <f>18*Lower.dat!B8*COS(RADIANS(26))</f>
-        <v>-0.44728104248987471</v>
+        <f>18*Lower.dat!B8*COS(RADIANS(47))</f>
+        <v>-0.33939358935584657</v>
       </c>
       <c r="C8">
-        <f>-Lower.dat!B8*SIN(RADIANS(26))+4</f>
-        <v>4.0121196411483346</v>
+        <f>-Lower.dat!B8*SIN(RADIANS(47))+4</f>
+        <v>4.0202197258671211</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4017,12 +4017,12 @@
         <v>48.664428599999994</v>
       </c>
       <c r="B9">
-        <f>18*Lower.dat!B9*COS(RADIANS(26))</f>
-        <v>-0.50329682125562258</v>
+        <f>18*Lower.dat!B9*COS(RADIANS(47))</f>
+        <v>-0.38189795330125242</v>
       </c>
       <c r="C9">
-        <f>-Lower.dat!B9*SIN(RADIANS(26))+4</f>
-        <v>4.013637458969332</v>
+        <f>-Lower.dat!B9*SIN(RADIANS(47))+4</f>
+        <v>4.0227519675301515</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4031,12 +4031,12 @@
         <v>48.838130399999997</v>
       </c>
       <c r="B10">
-        <f>18*Lower.dat!B10*COS(RADIANS(26))</f>
-        <v>-0.55686542792778515</v>
+        <f>18*Lower.dat!B10*COS(RADIANS(47))</f>
+        <v>-0.4225454209293229</v>
       </c>
       <c r="C10">
-        <f>-Lower.dat!B10*SIN(RADIANS(26))+4</f>
-        <v>4.0150889675914474</v>
+        <f>-Lower.dat!B10*SIN(RADIANS(47))+4</f>
+        <v>4.0251735826649337</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4045,12 +4045,12 @@
         <v>49.030895999999998</v>
       </c>
       <c r="B11">
-        <f>18*Lower.dat!B11*COS(RADIANS(26))</f>
-        <v>-0.60780612224276487</v>
+        <f>18*Lower.dat!B11*COS(RADIANS(47))</f>
+        <v>-0.46119884784765985</v>
       </c>
       <c r="C11">
-        <f>-Lower.dat!B11*SIN(RADIANS(26))+4</f>
-        <v>4.0164692696304245</v>
+        <f>-Lower.dat!B11*SIN(RADIANS(47))+4</f>
+        <v>4.0274764007517367</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4059,12 +4059,12 @@
         <v>49.242273600000004</v>
       </c>
       <c r="B12">
-        <f>18*Lower.dat!B12*COS(RADIANS(26))</f>
-        <v>-0.65593336548766734</v>
+        <f>18*Lower.dat!B12*COS(RADIANS(47))</f>
+        <v>-0.4977174486355731</v>
       </c>
       <c r="C12">
-        <f>-Lower.dat!B12*SIN(RADIANS(26))+4</f>
-        <v>4.0177733376820006</v>
+        <f>-Lower.dat!B12*SIN(RADIANS(47))+4</f>
+        <v>4.0296520343527833</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4073,12 +4073,12 @@
         <v>49.4717682</v>
       </c>
       <c r="B13">
-        <f>18*Lower.dat!B13*COS(RADIANS(26))</f>
-        <v>-0.70107137484845539</v>
+        <f>18*Lower.dat!B13*COS(RADIANS(47))</f>
+        <v>-0.53196784057719548</v>
       </c>
       <c r="C13">
-        <f>-Lower.dat!B13*SIN(RADIANS(26))+4</f>
-        <v>4.0189964086902368</v>
+        <f>-Lower.dat!B13*SIN(RADIANS(47))+4</f>
+        <v>4.0316925370541323</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4087,12 +4087,12 @@
         <v>49.718846999999997</v>
       </c>
       <c r="B14">
-        <f>18*Lower.dat!B14*COS(RADIANS(26))</f>
-        <v>-0.7430460281481378</v>
+        <f>18*Lower.dat!B14*COS(RADIANS(47))</f>
+        <v>-0.56381790103592588</v>
       </c>
       <c r="C14">
-        <f>-Lower.dat!B14*SIN(RADIANS(26))+4</f>
-        <v>4.0201337645962374</v>
+        <f>-Lower.dat!B14*SIN(RADIANS(47))+4</f>
+        <v>4.033590037512373</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4101,12 +4101,12 @@
         <v>49.982930400000001</v>
       </c>
       <c r="B15">
-        <f>18*Lower.dat!B15*COS(RADIANS(26))</f>
-        <v>-0.78170105233192777</v>
+        <f>18*Lower.dat!B15*COS(RADIANS(47))</f>
+        <v>-0.5931490511587717</v>
       </c>
       <c r="C15">
-        <f>-Lower.dat!B15*SIN(RADIANS(26))+4</f>
-        <v>4.0211811709854723</v>
+        <f>-Lower.dat!B15*SIN(RADIANS(47))+4</f>
+        <v>4.0353374712690835</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4115,12 +4115,12 @@
         <v>50.263402799999994</v>
       </c>
       <c r="B16">
-        <f>18*Lower.dat!B16*COS(RADIANS(26))</f>
-        <v>-0.81688830426075287</v>
+        <f>18*Lower.dat!B16*COS(RADIANS(47))</f>
+        <v>-0.61984888101342672</v>
       </c>
       <c r="C16">
-        <f>-Lower.dat!B16*SIN(RADIANS(26))+4</f>
-        <v>4.022134613733682</v>
+        <f>-Lower.dat!B16*SIN(RADIANS(47))+4</f>
+        <v>4.036928141385701</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4129,12 +4129,12 @@
         <v>50.559608999999995</v>
       </c>
       <c r="B17">
-        <f>18*Lower.dat!B17*COS(RADIANS(26))</f>
-        <v>-0.84848557091030152</v>
+        <f>18*Lower.dat!B17*COS(RADIANS(47))</f>
+        <v>-0.64382465624934426</v>
       </c>
       <c r="C17">
-        <f>-Lower.dat!B17*SIN(RADIANS(26))+4</f>
-        <v>4.0229907813256034</v>
+        <f>-Lower.dat!B17*SIN(RADIANS(47))+4</f>
+        <v>4.0383565231168994</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4143,12 +4143,12 @@
         <v>50.870857799999996</v>
       </c>
       <c r="B18">
-        <f>18*Lower.dat!B18*COS(RADIANS(26))</f>
-        <v>-0.87638685831839436</v>
+        <f>18*Lower.dat!B18*COS(RADIANS(47))</f>
+        <v>-0.66499594942190499</v>
       </c>
       <c r="C18">
-        <f>-Lower.dat!B18*SIN(RADIANS(26))+4</f>
-        <v>4.0237468017218188</v>
+        <f>-Lower.dat!B18*SIN(RADIANS(47))+4</f>
+        <v>4.0396178249140675</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4157,12 +4157,12 @@
         <v>51.196420200000006</v>
       </c>
       <c r="B19">
-        <f>18*Lower.dat!B19*COS(RADIANS(26))</f>
-        <v>-0.90051371842843086</v>
+        <f>18*Lower.dat!B19*COS(RADIANS(47))</f>
+        <v>-0.68330323471852483</v>
       </c>
       <c r="C19">
-        <f>-Lower.dat!B19*SIN(RADIANS(26))+4</f>
-        <v>4.0244005492737873</v>
+        <f>-Lower.dat!B19*SIN(RADIANS(47))+4</f>
+        <v>4.040708500465044</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4171,12 +4171,12 @@
         <v>51.5355366</v>
       </c>
       <c r="B20">
-        <f>18*Lower.dat!B20*COS(RADIANS(26))</f>
-        <v>-0.92081200527696394</v>
+        <f>18*Lower.dat!B20*COS(RADIANS(47))</f>
+        <v>-0.69870542657747037</v>
       </c>
       <c r="C20">
-        <f>-Lower.dat!B20*SIN(RADIANS(26))+4</f>
-        <v>4.0249505568286805</v>
+        <f>-Lower.dat!B20*SIN(RADIANS(47))+4</f>
+        <v>4.041626102054785</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -4185,12 +4185,12 @@
         <v>51.887416799999997</v>
       </c>
       <c r="B21">
-        <f>18*Lower.dat!B21*COS(RADIANS(26))</f>
-        <v>-0.93725187499370022</v>
+        <f>18*Lower.dat!B21*COS(RADIANS(47))</f>
+        <v>-0.71117987968785878</v>
       </c>
       <c r="C21">
-        <f>-Lower.dat!B21*SIN(RADIANS(26))+4</f>
-        <v>4.0253960157293829</v>
+        <f>-Lower.dat!B21*SIN(RADIANS(47))+4</f>
+        <v>4.0423692805653539</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4199,12 +4199,12 @@
         <v>52.251238200000003</v>
       </c>
       <c r="B22">
-        <f>18*Lower.dat!B22*COS(RADIANS(26))</f>
-        <v>-0.94983587698638083</v>
+        <f>18*Lower.dat!B22*COS(RADIANS(47))</f>
+        <v>-0.72072852852167035</v>
       </c>
       <c r="C22">
-        <f>-Lower.dat!B22*SIN(RADIANS(26))+4</f>
-        <v>4.0257369950552944</v>
+        <f>-Lower.dat!B22*SIN(RADIANS(47))+4</f>
+        <v>4.0429381512449316</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4213,12 +4213,12 @@
         <v>52.626149400000003</v>
       </c>
       <c r="B23">
-        <f>18*Lower.dat!B23*COS(RADIANS(26))</f>
-        <v>-0.95859086071743516</v>
+        <f>18*Lower.dat!B23*COS(RADIANS(47))</f>
+        <v>-0.72737174625496359</v>
       </c>
       <c r="C23">
-        <f>-Lower.dat!B23*SIN(RADIANS(26))+4</f>
-        <v>4.025974222326294</v>
+        <f>-Lower.dat!B23*SIN(RADIANS(47))+4</f>
+        <v>4.0433339278466578</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4227,12 +4227,12 @@
         <v>53.011275600000005</v>
       </c>
       <c r="B24">
-        <f>18*Lower.dat!B24*COS(RADIANS(26))</f>
-        <v>-0.96356958741787058</v>
+        <f>18*Lower.dat!B24*COS(RADIANS(47))</f>
+        <v>-0.7311495677246066</v>
       </c>
       <c r="C24">
-        <f>-Lower.dat!B24*SIN(RADIANS(26))+4</f>
-        <v>4.0261091271741476</v>
+        <f>-Lower.dat!B24*SIN(RADIANS(47))+4</f>
+        <v>4.0435589954875519</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4241,12 +4241,12 @@
         <v>53.4057186</v>
       </c>
       <c r="B25">
-        <f>18*Lower.dat!B25*COS(RADIANS(26))</f>
-        <v>-0.96485396574583726</v>
+        <f>18*Lower.dat!B25*COS(RADIANS(47))</f>
+        <v>-0.73212414462237296</v>
       </c>
       <c r="C25">
-        <f>-Lower.dat!B25*SIN(RADIANS(26))+4</f>
-        <v>4.0261439290167367</v>
+        <f>-Lower.dat!B25*SIN(RADIANS(47))+4</f>
+        <v>4.0436170569192562</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4255,12 +4255,12 @@
         <v>53.808556800000005</v>
       </c>
       <c r="B26">
-        <f>18*Lower.dat!B26*COS(RADIANS(26))</f>
-        <v>-0.962546962640213</v>
+        <f>18*Lower.dat!B26*COS(RADIANS(47))</f>
+        <v>-0.73037360750970148</v>
       </c>
       <c r="C26">
-        <f>-Lower.dat!B26*SIN(RADIANS(26))+4</f>
-        <v>4.0260814178724846</v>
+        <f>-Lower.dat!B26*SIN(RADIANS(47))+4</f>
+        <v>4.0435127668511806</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4269,12 +4269,12 @@
         <v>54.218846999999997</v>
       </c>
       <c r="B27">
-        <f>18*Lower.dat!B27*COS(RADIANS(26))</f>
-        <v>-0.95677421911142047</v>
+        <f>18*Lower.dat!B27*COS(RADIANS(47))</f>
+        <v>-0.72599329186797157</v>
       </c>
       <c r="C27">
-        <f>-Lower.dat!B27*SIN(RADIANS(26))+4</f>
-        <v>4.0259249981422389</v>
+        <f>-Lower.dat!B27*SIN(RADIANS(47))+4</f>
+        <v>4.0432518049937238</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4283,12 +4283,12 @@
         <v>54.635633400000003</v>
       </c>
       <c r="B28">
-        <f>18*Lower.dat!B28*COS(RADIANS(26))</f>
-        <v>-0.94768242221982102</v>
+        <f>18*Lower.dat!B28*COS(RADIANS(47))</f>
+        <v>-0.7190945027675949</v>
       </c>
       <c r="C28">
-        <f>-Lower.dat!B28*SIN(RADIANS(26))+4</f>
-        <v>4.0256786444959802</v>
+        <f>-Lower.dat!B28*SIN(RADIANS(47))+4</f>
+        <v>4.0428408024621518</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -4297,12 +4297,12 @@
         <v>55.057942199999999</v>
       </c>
       <c r="B29">
-        <f>18*Lower.dat!B29*COS(RADIANS(26))</f>
-        <v>-0.9354360755325406</v>
+        <f>18*Lower.dat!B29*COS(RADIANS(47))</f>
+        <v>-0.7098020643142342</v>
       </c>
       <c r="C29">
-        <f>-Lower.dat!B29*SIN(RADIANS(26))+4</f>
-        <v>4.0253468143642985</v>
+        <f>-Lower.dat!B29*SIN(RADIANS(47))+4</f>
+        <v>4.0422871957823059</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4311,12 +4311,12 @@
         <v>55.484786999999997</v>
       </c>
       <c r="B30">
-        <f>18*Lower.dat!B30*COS(RADIANS(26))</f>
-        <v>-0.9202110216909436</v>
+        <f>18*Lower.dat!B30*COS(RADIANS(47))</f>
+        <v>-0.6982494046202955</v>
       </c>
       <c r="C30">
-        <f>-Lower.dat!B30*SIN(RADIANS(26))+4</f>
-        <v>4.0249342724242307</v>
+        <f>-Lower.dat!B30*SIN(RADIANS(47))+4</f>
+        <v>4.0415989340726757</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -4325,12 +4325,12 @@
         <v>55.915170599999996</v>
       </c>
       <c r="B31">
-        <f>18*Lower.dat!B31*COS(RADIANS(26))</f>
-        <v>-0.90219767603073353</v>
+        <f>18*Lower.dat!B31*COS(RADIANS(47))</f>
+        <v>-0.68458100945225164</v>
       </c>
       <c r="C31">
-        <f>-Lower.dat!B31*SIN(RADIANS(26))+4</f>
-        <v>4.0244461782182537</v>
+        <f>-Lower.dat!B31*SIN(RADIANS(47))+4</f>
+        <v>4.040784625222984</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4339,12 +4339,12 @@
         <v>56.348086800000004</v>
       </c>
       <c r="B32">
-        <f>18*Lower.dat!B32*COS(RADIANS(26))</f>
-        <v>-0.88159617105563848</v>
+        <f>18*Lower.dat!B32*COS(RADIANS(47))</f>
+        <v>-0.66894873789272513</v>
       </c>
       <c r="C32">
-        <f>-Lower.dat!B32*SIN(RADIANS(26))+4</f>
-        <v>4.0238879545877069</v>
+        <f>-Lower.dat!B32*SIN(RADIANS(47))+4</f>
+        <v>4.0398533163959254</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4353,12 +4353,12 @@
         <v>56.782525800000002</v>
       </c>
       <c r="B33">
-        <f>18*Lower.dat!B33*COS(RADIANS(26))</f>
-        <v>-0.85861149683416638</v>
+        <f>18*Lower.dat!B33*COS(RADIANS(47))</f>
+        <v>-0.6515081349090277</v>
       </c>
       <c r="C33">
-        <f>-Lower.dat!B33*SIN(RADIANS(26))+4</f>
-        <v>4.0232651559957411</v>
+        <f>-Lower.dat!B33*SIN(RADIANS(47))+4</f>
+        <v>4.0388142743446096</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4367,12 +4367,12 @@
         <v>57.217474199999998</v>
       </c>
       <c r="B34">
-        <f>18*Lower.dat!B34*COS(RADIANS(26))</f>
-        <v>-0.83345350099960469</v>
+        <f>18*Lower.dat!B34*COS(RADIANS(47))</f>
+        <v>-0.63241843135315967</v>
       </c>
       <c r="C34">
-        <f>-Lower.dat!B34*SIN(RADIANS(26))+4</f>
-        <v>4.0225834685273227</v>
+        <f>-Lower.dat!B34*SIN(RADIANS(47))+4</f>
+        <v>4.0376769854125572</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4381,12 +4381,12 @@
         <v>57.651913199999996</v>
       </c>
       <c r="B35">
-        <f>18*Lower.dat!B35*COS(RADIANS(26))</f>
-        <v>-0.80633365512991939</v>
+        <f>18*Lower.dat!B35*COS(RADIANS(47))</f>
+        <v>-0.61184009031448661</v>
       </c>
       <c r="C35">
-        <f>-Lower.dat!B35*SIN(RADIANS(26))+4</f>
-        <v>4.0218486222702383</v>
+        <f>-Lower.dat!B35*SIN(RADIANS(47))+4</f>
+        <v>4.0364510093551074</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4395,12 +4395,12 @@
         <v>58.084829400000004</v>
       </c>
       <c r="B36">
-        <f>18*Lower.dat!B36*COS(RADIANS(26))</f>
-        <v>-0.77746342468768126</v>
+        <f>18*Lower.dat!B36*COS(RADIANS(47))</f>
+        <v>-0.58993357024205717</v>
       </c>
       <c r="C36">
-        <f>-Lower.dat!B36*SIN(RADIANS(26))+4</f>
-        <v>4.0210663471465669</v>
+        <f>-Lower.dat!B36*SIN(RADIANS(47))+4</f>
+        <v>4.0351459056511514</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -4409,12 +4409,12 @@
         <v>58.515214799999995</v>
       </c>
       <c r="B37">
-        <f>18*Lower.dat!B37*COS(RADIANS(26))</f>
-        <v>-0.74705426902006666</v>
+        <f>18*Lower.dat!B37*COS(RADIANS(47))</f>
+        <v>-0.56685932494460289</v>
       </c>
       <c r="C37">
-        <f>-Lower.dat!B37*SIN(RADIANS(26))+4</f>
-        <v>4.0202423729126853</v>
+        <f>-Lower.dat!B37*SIN(RADIANS(47))+4</f>
+        <v>4.0337712335031277</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -4423,12 +4423,12 @@
         <v>58.942057800000001</v>
       </c>
       <c r="B38">
-        <f>18*Lower.dat!B38*COS(RADIANS(26))</f>
-        <v>-0.71531118023404849</v>
+        <f>18*Lower.dat!B38*COS(RADIANS(47))</f>
+        <v>-0.542772900936208</v>
       </c>
       <c r="C38">
-        <f>-Lower.dat!B38*SIN(RADIANS(26))+4</f>
-        <v>4.019382254086981</v>
+        <f>-Lower.dat!B38*SIN(RADIANS(47))+4</f>
+        <v>4.0323362597562955</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4437,12 +4437,12 @@
         <v>59.364366599999997</v>
       </c>
       <c r="B39">
-        <f>18*Lower.dat!B39*COS(RADIANS(26))</f>
-        <v>-0.6824375101842024</v>
+        <f>18*Lower.dat!B39*COS(RADIANS(47))</f>
+        <v>-0.51782860011941312</v>
       </c>
       <c r="C39">
-        <f>-Lower.dat!B39*SIN(RADIANS(26))+4</f>
-        <v>4.0184915007431439</v>
+        <f>-Lower.dat!B39*SIN(RADIANS(47))+4</f>
+        <v>4.0308501771068856</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -4451,12 +4451,12 @@
         <v>59.781153000000003</v>
       </c>
       <c r="B40">
-        <f>18*Lower.dat!B40*COS(RADIANS(26))</f>
-        <v>-0.64863175316032384</v>
+        <f>18*Lower.dat!B40*COS(RADIANS(47))</f>
+        <v>-0.49217703851206984</v>
       </c>
       <c r="C40">
-        <f>-Lower.dat!B40*SIN(RADIANS(26))+4</f>
-        <v>4.0175754913330497</v>
+        <f>-Lower.dat!B40*SIN(RADIANS(47))+4</f>
+        <v>4.0293219586607201</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -4465,12 +4465,12 @@
         <v>60.191445000000002</v>
       </c>
       <c r="B41">
-        <f>18*Lower.dat!B41*COS(RADIANS(26))</f>
-        <v>-0.61408753161817464</v>
+        <f>18*Lower.dat!B41*COS(RADIANS(47))</f>
+        <v>-0.46596513541993506</v>
       </c>
       <c r="C41">
-        <f>-Lower.dat!B41*SIN(RADIANS(26))+4</f>
-        <v>4.0166394723001195</v>
+        <f>-Lower.dat!B41*SIN(RADIANS(47))+4</f>
+        <v>4.0277603572881526</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -4479,12 +4479,12 @@
         <v>60.5942814</v>
       </c>
       <c r="B42">
-        <f>18*Lower.dat!B42*COS(RADIANS(26))</f>
-        <v>-0.57899522012416038</v>
+        <f>18*Lower.dat!B42*COS(RADIANS(47))</f>
+        <v>-0.43933734567403604</v>
       </c>
       <c r="C42">
-        <f>-Lower.dat!B42*SIN(RADIANS(26))+4</f>
-        <v>4.0156886020821343</v>
+        <f>-Lower.dat!B42*SIN(RADIANS(47))+4</f>
+        <v>4.0261739790358959</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -4493,12 +4493,12 @@
         <v>60.988724399999995</v>
       </c>
       <c r="B43">
-        <f>18*Lower.dat!B43*COS(RADIANS(26))</f>
-        <v>-0.54353545976894313</v>
+        <f>18*Lower.dat!B43*COS(RADIANS(47))</f>
+        <v>-0.41243073841507139</v>
       </c>
       <c r="C43">
-        <f>-Lower.dat!B43*SIN(RADIANS(26))+4</f>
-        <v>4.0147277753761355</v>
+        <f>-Lower.dat!B43*SIN(RADIANS(47))+4</f>
+        <v>4.0245709899404831</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -4507,12 +4507,12 @@
         <v>61.373850599999997</v>
       </c>
       <c r="B44">
-        <f>18*Lower.dat!B44*COS(RADIANS(26))</f>
-        <v>-0.50788887533546534</v>
+        <f>18*Lower.dat!B44*COS(RADIANS(47))</f>
+        <v>-0.38538237040956141</v>
       </c>
       <c r="C44">
-        <f>-Lower.dat!B44*SIN(RADIANS(26))+4</f>
-        <v>4.0137618864372868</v>
+        <f>-Lower.dat!B44*SIN(RADIANS(47))+4</f>
+        <v>4.0229595553012416</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -4521,12 +4521,12 @@
         <v>61.748763600000004</v>
       </c>
       <c r="B45">
-        <f>18*Lower.dat!B45*COS(RADIANS(26))</f>
-        <v>-0.47222958971256318</v>
+        <f>18*Lower.dat!B45*COS(RADIANS(47))</f>
+        <v>-0.35832436483425006</v>
       </c>
       <c r="C45">
-        <f>-Lower.dat!B45*SIN(RADIANS(26))+4</f>
-        <v>4.0127956533437725</v>
+        <f>-Lower.dat!B45*SIN(RADIANS(47))+4</f>
+        <v>4.0213475464937618</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -4535,12 +4535,12 @@
         <v>62.112583200000003</v>
       </c>
       <c r="B46">
-        <f>18*Lower.dat!B46*COS(RADIANS(26))</f>
-        <v>-0.43673170744288825</v>
+        <f>18*Lower.dat!B46*COS(RADIANS(47))</f>
+        <v>-0.33138883094493043</v>
       </c>
       <c r="C46">
-        <f>-Lower.dat!B46*SIN(RADIANS(26))+4</f>
-        <v>4.0118337936766615</v>
+        <f>-Lower.dat!B46*SIN(RADIANS(47))+4</f>
+        <v>4.019742834064278</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -4549,12 +4549,12 @@
         <v>62.4644634</v>
       </c>
       <c r="B47">
-        <f>18*Lower.dat!B47*COS(RADIANS(26))</f>
-        <v>-0.40156444085040965</v>
+        <f>18*Lower.dat!B47*COS(RADIANS(47))</f>
+        <v>-0.30470416581757831</v>
       </c>
       <c r="C47">
-        <f>-Lower.dat!B47*SIN(RADIANS(26))+4</f>
-        <v>4.0108808924562211</v>
+        <f>-Lower.dat!B47*SIN(RADIANS(47))+4</f>
+        <v>4.0181530674020527</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -4563,12 +4563,12 @@
         <v>62.803579799999994</v>
       </c>
       <c r="B48">
-        <f>18*Lower.dat!B48*COS(RADIANS(26))</f>
-        <v>-0.3668905064803839</v>
+        <f>18*Lower.dat!B48*COS(RADIANS(47))</f>
+        <v>-0.27839383757870939</v>
       </c>
       <c r="C48">
-        <f>-Lower.dat!B48*SIN(RADIANS(26))+4</f>
-        <v>4.0099413586914396</v>
+        <f>-Lower.dat!B48*SIN(RADIANS(47))+4</f>
+        <v>4.0165856022490614</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4577,12 +4577,12 @@
         <v>63.129142200000004</v>
       </c>
       <c r="B49">
-        <f>18*Lower.dat!B49*COS(RADIANS(26))</f>
-        <v>-0.33287905346436802</v>
+        <f>18*Lower.dat!B49*COS(RADIANS(47))</f>
+        <v>-0.2525861953543585</v>
       </c>
       <c r="C49">
-        <f>-Lower.dat!B49*SIN(RADIANS(26))+4</f>
-        <v>4.009019775690307</v>
+        <f>-Lower.dat!B49*SIN(RADIANS(47))+4</f>
+        <v>4.0150480851378996</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4591,12 +4591,12 @@
         <v>63.440391000000005</v>
       </c>
       <c r="B50">
-        <f>18*Lower.dat!B50*COS(RADIANS(26))</f>
-        <v>-0.29969110713359903</v>
+        <f>18*Lower.dat!B50*COS(RADIANS(47))</f>
+        <v>-0.22740342399019128</v>
       </c>
       <c r="C50">
-        <f>-Lower.dat!B50*SIN(RADIANS(26))+4</f>
-        <v>4.0081205066362466</v>
+        <f>-Lower.dat!B50*SIN(RADIANS(47))+4</f>
+        <v>4.013547795357753</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -4605,12 +4605,12 @@
         <v>63.736597200000006</v>
       </c>
       <c r="B51">
-        <f>18*Lower.dat!B51*COS(RADIANS(26))</f>
-        <v>-0.26748765816541076</v>
+        <f>18*Lower.dat!B51*COS(RADIANS(47))</f>
+        <v>-0.20296768203674448</v>
       </c>
       <c r="C51">
-        <f>-Lower.dat!B51*SIN(RADIANS(26))+4</f>
-        <v>4.0072479137736909</v>
+        <f>-Lower.dat!B51*SIN(RADIANS(47))+4</f>
+        <v>4.012092010631247</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -4619,12 +4619,12 @@
         <v>64.017069599999999</v>
       </c>
       <c r="B52">
-        <f>18*Lower.dat!B52*COS(RADIANS(26))</f>
-        <v>-0.23642803660009076</v>
+        <f>18*Lower.dat!B52*COS(RADIANS(47))</f>
+        <v>-0.17939986796528884</v>
       </c>
       <c r="C52">
-        <f>-Lower.dat!B52*SIN(RADIANS(26))+4</f>
-        <v>4.0064063143500279</v>
+        <f>-Lower.dat!B52*SIN(RADIANS(47))+4</f>
+        <v>4.0106879336104742</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -4633,12 +4633,12 @@
         <v>64.281153000000003</v>
       </c>
       <c r="B53">
-        <f>18*Lower.dat!B53*COS(RADIANS(26))</f>
-        <v>-0.20667153170862884</v>
+        <f>18*Lower.dat!B53*COS(RADIANS(47))</f>
+        <v>-0.15682084931164963</v>
       </c>
       <c r="C53">
-        <f>-Lower.dat!B53*SIN(RADIANS(26))+4</f>
-        <v>4.0056000245079515</v>
+        <f>-Lower.dat!B53*SIN(RADIANS(47))+4</f>
+        <v>4.0093427651045168</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -4647,12 +4647,12 @@
         <v>64.5282318</v>
       </c>
       <c r="B54">
-        <f>18*Lower.dat!B54*COS(RADIANS(26))</f>
-        <v>-0.17837091659865353</v>
+        <f>18*Lower.dat!B54*COS(RADIANS(47))</f>
+        <v>-0.1353465491944694</v>
       </c>
       <c r="C54">
-        <f>-Lower.dat!B54*SIN(RADIANS(26))+4</f>
-        <v>4.0048331838265296</v>
+        <f>-Lower.dat!B54*SIN(RADIANS(47))+4</f>
+        <v>4.0080634113536648</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -4661,12 +4661,12 @@
         <v>64.757728200000003</v>
       </c>
       <c r="B55">
-        <f>18*Lower.dat!B55*COS(RADIANS(26))</f>
-        <v>-0.15167892157003057</v>
+        <f>18*Lower.dat!B55*COS(RADIANS(47))</f>
+        <v>-0.11509285825017268</v>
       </c>
       <c r="C55">
-        <f>-Lower.dat!B55*SIN(RADIANS(26))+4</f>
-        <v>4.0041099307249013</v>
+        <f>-Lower.dat!B55*SIN(RADIANS(47))+4</f>
+        <v>4.0068567766630441</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -4675,12 +4675,12 @@
         <v>64.969104000000002</v>
       </c>
       <c r="B56">
-        <f>18*Lower.dat!B56*COS(RADIANS(26))</f>
-        <v>-0.126738525100698</v>
+        <f>18*Lower.dat!B56*COS(RADIANS(47))</f>
+        <v>-9.6168267503905405E-2</v>
       </c>
       <c r="C56">
-        <f>-Lower.dat!B56*SIN(RADIANS(26))+4</f>
-        <v>4.0034341393843542</v>
+        <f>-Lower.dat!B56*SIN(RADIANS(47))+4</f>
+        <v>4.0057293244982484</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -4689,12 +4689,12 @@
         <v>65.161869600000003</v>
       </c>
       <c r="B57">
-        <f>18*Lower.dat!B57*COS(RADIANS(26))</f>
-        <v>-0.10369426845932486</v>
+        <f>18*Lower.dat!B57*COS(RADIANS(47))</f>
+        <v>-7.8682453815009823E-2</v>
       </c>
       <c r="C57">
-        <f>-Lower.dat!B57*SIN(RADIANS(26))+4</f>
-        <v>4.0028097263319502</v>
+        <f>-Lower.dat!B57*SIN(RADIANS(47))+4</f>
+        <v>4.0046875889721765</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -4703,12 +4703,12 @@
         <v>65.335571399999992</v>
       </c>
       <c r="B58">
-        <f>18*Lower.dat!B58*COS(RADIANS(26))</f>
-        <v>-8.2676091681732317E-2</v>
+        <f>18*Lower.dat!B58*COS(RADIANS(47))</f>
+        <v>-6.2734014733949697E-2</v>
       </c>
       <c r="C58">
-        <f>-Lower.dat!B58*SIN(RADIANS(26))+4</f>
-        <v>4.0022402124560248</v>
+        <f>-Lower.dat!B58*SIN(RADIANS(47))+4</f>
+        <v>4.0037374441363838</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -4717,12 +4717,12 @@
         <v>65.489806200000004</v>
       </c>
       <c r="B59">
-        <f>18*Lower.dat!B59*COS(RADIANS(26))</f>
-        <v>-6.381064206815773E-2</v>
+        <f>18*Lower.dat!B59*COS(RADIANS(47))</f>
+        <v>-4.8419049307468667E-2</v>
       </c>
       <c r="C59">
-        <f>-Lower.dat!B59*SIN(RADIANS(26))+4</f>
-        <v>4.0017290294241086</v>
+        <f>-Lower.dat!B59*SIN(RADIANS(47))+4</f>
+        <v>4.002884615191471</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -4731,12 +4731,12 @@
         <v>65.624212200000002</v>
       </c>
       <c r="B60">
-        <f>18*Lower.dat!B60*COS(RADIANS(26))</f>
-        <v>-4.7211577399879044E-2</v>
+        <f>18*Lower.dat!B60*COS(RADIANS(47))</f>
+        <v>-3.5823800230162989E-2</v>
       </c>
       <c r="C60">
-        <f>-Lower.dat!B60*SIN(RADIANS(26))+4</f>
-        <v>4.0012792569364182</v>
+        <f>-Lower.dat!B60*SIN(RADIANS(47))+4</f>
+        <v>4.0021342401356108</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -4745,12 +4745,12 @@
         <v>65.738476200000008</v>
       </c>
       <c r="B61">
-        <f>18*Lower.dat!B61*COS(RADIANS(26))</f>
-        <v>-3.2982793443922041E-2</v>
+        <f>18*Lower.dat!B61*COS(RADIANS(47))</f>
+        <v>-2.5027102851488712E-2</v>
       </c>
       <c r="C61">
-        <f>-Lower.dat!B61*SIN(RADIANS(26))+4</f>
-        <v>4.0008937101791409</v>
+        <f>-Lower.dat!B61*SIN(RADIANS(47))+4</f>
+        <v>4.0014910156666952</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -4759,12 +4759,12 @@
         <v>65.832329999999999</v>
       </c>
       <c r="B62">
-        <f>18*Lower.dat!B62*COS(RADIANS(26))</f>
-        <v>-2.1213574542139974E-2</v>
+        <f>18*Lower.dat!B62*COS(RADIANS(47))</f>
+        <v>-1.6096705478161819E-2</v>
       </c>
       <c r="C62">
-        <f>-Lower.dat!B62*SIN(RADIANS(26))+4</f>
-        <v>4.0005748084235648</v>
+        <f>-Lower.dat!B62*SIN(RADIANS(47))+4</f>
+        <v>4.000958977960515</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -4773,12 +4773,12 @@
         <v>65.905557600000009</v>
       </c>
       <c r="B63">
-        <f>18*Lower.dat!B63*COS(RADIANS(26))</f>
-        <v>-1.1978585457354056E-2</v>
+        <f>18*Lower.dat!B63*COS(RADIANS(47))</f>
+        <v>-9.0892631870691659E-3</v>
       </c>
       <c r="C63">
-        <f>-Lower.dat!B63*SIN(RADIANS(26))+4</f>
-        <v>4.0003245748051377</v>
+        <f>-Lower.dat!B63*SIN(RADIANS(47))+4</f>
+        <v>4.0005415023021662</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -4787,12 +4787,12 @@
         <v>65.957984400000001</v>
       </c>
       <c r="B64">
-        <f>18*Lower.dat!B64*COS(RADIANS(26))</f>
-        <v>-5.3378836041428216E-3</v>
+        <f>18*Lower.dat!B64*COS(RADIANS(47))</f>
+        <v>-4.0503471059021379E-3</v>
       </c>
       <c r="C64">
-        <f>-Lower.dat!B64*SIN(RADIANS(26))+4</f>
-        <v>4.0001446366548725</v>
+        <f>-Lower.dat!B64*SIN(RADIANS(47))+4</f>
+        <v>4.0002413036389504</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -4801,12 +4801,12 @@
         <v>65.989489800000001</v>
       </c>
       <c r="B65">
-        <f>18*Lower.dat!B65*COS(RADIANS(26))</f>
-        <v>-1.3369047795878518E-3</v>
+        <f>18*Lower.dat!B65*COS(RADIANS(47))</f>
+        <v>-1.0144335857506846E-3</v>
       </c>
       <c r="C65">
-        <f>-Lower.dat!B65*SIN(RADIANS(26))+4</f>
-        <v>4.0000362251127122</v>
+        <f>-Lower.dat!B65*SIN(RADIANS(47))+4</f>
+        <v>4.0000604359353202</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -4815,11 +4815,11 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <f>18*Lower.dat!B66*COS(RADIANS(26))</f>
+        <f>18*Lower.dat!B66*COS(RADIANS(47))</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f>-Lower.dat!B66*SIN(RADIANS(26))+4</f>
+        <f>-Lower.dat!B66*SIN(RADIANS(47))+4</f>
         <v>4</v>
       </c>
     </row>
@@ -4845,12 +4845,12 @@
         <v>51</v>
       </c>
       <c r="B1">
-        <f>12*Lower.dat!B1*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4523094954143154</v>
+        <f>12*Lower.dat!B1*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.940611048575114</v>
       </c>
       <c r="C1">
-        <f>4+-12*Lower.dat!B1*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.279498787085842</v>
+        <f>4+-12*Lower.dat!B1*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.459950801874953</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4859,12 +4859,12 @@
         <v>51.007006799999999</v>
       </c>
       <c r="B2">
-        <f>12*Lower.dat!B2*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4063678431732907</v>
+        <f>12*Lower.dat!B2*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.905750858283522</v>
       </c>
       <c r="C2">
-        <f>4+-12*Lower.dat!B2*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.301906028056347</v>
+        <f>4+-12*Lower.dat!B2*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.497333779169164</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4873,12 +4873,12 @@
         <v>51.028010399999999</v>
       </c>
       <c r="B3">
-        <f>12*Lower.dat!B3*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3614310750038534</v>
+        <f>12*Lower.dat!B3*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.871653166688596</v>
       </c>
       <c r="C3">
-        <f>4+-12*Lower.dat!B3*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.323823154317409</v>
+        <f>4+-12*Lower.dat!B3*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.533899076719635</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4887,12 +4887,12 @@
         <v>51.062961599999994</v>
       </c>
       <c r="B4">
-        <f>12*Lower.dat!B4*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3175498271721731</v>
+        <f>12*Lower.dat!B4*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.8383563962194</v>
       </c>
       <c r="C4">
-        <f>4+-12*Lower.dat!B4*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.345225468911856</v>
+        <f>4+-12*Lower.dat!B4*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.569605491515674</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4901,12 +4901,12 @@
         <v>51.111778799999996</v>
       </c>
       <c r="B5">
-        <f>12*Lower.dat!B5*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2747919560977419</v>
+        <f>12*Lower.dat!B5*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.805912035831614</v>
       </c>
       <c r="C5">
-        <f>4+-12*Lower.dat!B5*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.366079876052556</v>
+        <f>4+-12*Lower.dat!B5*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.604397808412298</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4915,12 +4915,12 @@
         <v>51.174349199999995</v>
       </c>
       <c r="B6">
-        <f>12*Lower.dat!B6*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2332371469480714</v>
+        <f>12*Lower.dat!B6*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.774380550048548</v>
       </c>
       <c r="C6">
-        <f>4+-12*Lower.dat!B6*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.386347510686484</v>
+        <f>4+-12*Lower.dat!B6*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.638211187146645</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4929,12 +4929,12 @@
         <v>51.250525199999998</v>
       </c>
       <c r="B7">
-        <f>12*Lower.dat!B7*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1929790666674727</v>
+        <f>12*Lower.dat!B7*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.743833012663668</v>
       </c>
       <c r="C7">
-        <f>4+-12*Lower.dat!B7*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.405982688392434</v>
+        <f>4+-12*Lower.dat!B7*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.670969410406499</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4943,12 +4943,12 @@
         <v>51.340129200000007</v>
       </c>
       <c r="B8">
-        <f>12*Lower.dat!B8*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1541221337543988</v>
+        <f>12*Lower.dat!B8*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.714348655671216</v>
       </c>
       <c r="C8">
-        <f>4+-12*Lower.dat!B8*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.424934480865858</v>
+        <f>4+-12*Lower.dat!B8*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.702587512280402</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4957,12 +4957,12 @@
         <v>51.442952399999996</v>
       </c>
       <c r="B9">
-        <f>12*Lower.dat!B9*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1167782812439002</v>
+        <f>12*Lower.dat!B9*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.686012413040945</v>
       </c>
       <c r="C9">
-        <f>4+-12*Lower.dat!B9*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.443148294717822</v>
+        <f>4+-12*Lower.dat!B9*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.732974412236771</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4971,12 +4971,12 @@
         <v>51.558753600000003</v>
       </c>
       <c r="B10">
-        <f>12*Lower.dat!B10*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0810658767957921</v>
+        <f>12*Lower.dat!B10*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.6589141012889</v>
       </c>
       <c r="C10">
-        <f>4+-12*Lower.dat!B10*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.460566398183211</v>
+        <f>4+-12*Lower.dat!B10*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.762033793854162</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4985,12 +4985,12 @@
         <v>51.687263999999999</v>
       </c>
       <c r="B11">
-        <f>12*Lower.dat!B11*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0471054139191391</v>
+        <f>12*Lower.dat!B11*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.633145150010009</v>
       </c>
       <c r="C11">
-        <f>4+-12*Lower.dat!B11*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.477130022650936</v>
+        <f>4+-12*Lower.dat!B11*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.789667610895798</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4999,12 +4999,12 @@
         <v>51.828182400000003</v>
       </c>
       <c r="B12">
-        <f>12*Lower.dat!B12*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0150205850892036</v>
+        <f>12*Lower.dat!B12*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.608799416151399</v>
       </c>
       <c r="C12">
-        <f>4+-12*Lower.dat!B12*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.492778839269853</v>
+        <f>4+-12*Lower.dat!B12*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.815775214108356</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -5013,12 +5013,12 @@
         <v>51.981178799999995</v>
       </c>
       <c r="B13">
-        <f>12*Lower.dat!B13*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9849285788486783</v>
+        <f>12*Lower.dat!B13*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.585965821523651</v>
       </c>
       <c r="C13">
-        <f>4+-12*Lower.dat!B13*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.507455691368683</v>
+        <f>4+-12*Lower.dat!B13*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.840261246524541</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5027,12 +5027,12 @@
         <v>52.145898000000003</v>
       </c>
       <c r="B14">
-        <f>12*Lower.dat!B14*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9569454766488903</v>
+        <f>12*Lower.dat!B14*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.564732447884499</v>
       </c>
       <c r="C14">
-        <f>4+-12*Lower.dat!B14*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.521103962240687</v>
+        <f>4+-12*Lower.dat!B14*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.863031252023433</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5041,12 +5041,12 @@
         <v>52.321953600000001</v>
       </c>
       <c r="B15">
-        <f>12*Lower.dat!B15*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9311754605263634</v>
+        <f>12*Lower.dat!B15*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.545178347802601</v>
       </c>
       <c r="C15">
-        <f>4+-12*Lower.dat!B15*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.533672838911514</v>
+        <f>4+-12*Lower.dat!B15*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.884000457103951</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -5055,12 +5055,12 @@
         <v>52.508935199999996</v>
       </c>
       <c r="B16">
-        <f>12*Lower.dat!B16*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9077172925738139</v>
+        <f>12*Lower.dat!B16*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.527378461232828</v>
       </c>
       <c r="C16">
-        <f>4+-12*Lower.dat!B16*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.545114151890022</v>
+        <f>4+-12*Lower.dat!B16*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.903088498503362</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5069,12 +5069,12 @@
         <v>52.706406000000001</v>
       </c>
       <c r="B17">
-        <f>12*Lower.dat!B17*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8866524481407811</v>
+        <f>12*Lower.dat!B17*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.511394611075552</v>
       </c>
       <c r="C17">
-        <f>4+-12*Lower.dat!B17*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.555388162993083</v>
+        <f>4+-12*Lower.dat!B17*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.92022907927775</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5083,12 +5083,12 @@
         <v>52.913905200000002</v>
       </c>
       <c r="B18">
-        <f>12*Lower.dat!B18*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8680515898687196</v>
+        <f>12*Lower.dat!B18*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.497280415627177</v>
       </c>
       <c r="C18">
-        <f>4+-12*Lower.dat!B18*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.564460407747664</v>
+        <f>4+-12*Lower.dat!B18*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.935364700843756</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -5097,12 +5097,12 @@
         <v>53.130946800000004</v>
       </c>
       <c r="B19">
-        <f>12*Lower.dat!B19*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8519670164620283</v>
+        <f>12*Lower.dat!B19*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.485075558762766</v>
       </c>
       <c r="C19">
-        <f>4+-12*Lower.dat!B19*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.572305378371286</v>
+        <f>4+-12*Lower.dat!B19*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.948452807455485</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -5111,12 +5111,12 @@
         <v>53.3570244</v>
       </c>
       <c r="B20">
-        <f>12*Lower.dat!B20*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8384348252296725</v>
+        <f>12*Lower.dat!B20*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.474807430856799</v>
       </c>
       <c r="C20">
-        <f>4+-12*Lower.dat!B20*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.578905469030012</v>
+        <f>4+-12*Lower.dat!B20*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.959464026532373</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -5125,12 +5125,12 @@
         <v>53.591611200000003</v>
       </c>
       <c r="B21">
-        <f>12*Lower.dat!B21*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8274749120851821</v>
+        <f>12*Lower.dat!B21*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.466491128783208</v>
       </c>
       <c r="C21">
-        <f>4+-12*Lower.dat!B21*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.58425097583843</v>
+        <f>4+-12*Lower.dat!B21*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.968382168659204</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -5139,12 +5139,12 @@
         <v>53.834158799999997</v>
       </c>
       <c r="B22">
-        <f>12*Lower.dat!B22*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8190855774233947</v>
+        <f>12*Lower.dat!B22*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.460125362894001</v>
       </c>
       <c r="C22">
-        <f>4+-12*Lower.dat!B22*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.588342727749371</v>
+        <f>4+-12*Lower.dat!B22*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.975208616814136</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -5153,12 +5153,12 @@
         <v>54.084099600000002</v>
       </c>
       <c r="B23">
-        <f>12*Lower.dat!B23*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8132489216026917</v>
+        <f>12*Lower.dat!B23*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.455696551071807</v>
       </c>
       <c r="C23">
-        <f>4+-12*Lower.dat!B23*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.59118945500137</v>
+        <f>4+-12*Lower.dat!B23*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.979957936034843</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -5167,12 +5167,12 @@
         <v>54.340850399999994</v>
       </c>
       <c r="B24">
-        <f>12*Lower.dat!B24*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8099297704690684</v>
+        <f>12*Lower.dat!B24*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.453178003425375</v>
       </c>
       <c r="C24">
-        <f>4+-12*Lower.dat!B24*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.59280831317561</v>
+        <f>4+-12*Lower.dat!B24*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.98265874772558</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -5181,12 +5181,12 @@
         <v>54.603812399999995</v>
       </c>
       <c r="B25">
-        <f>12*Lower.dat!B25*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8090735182504236</v>
+        <f>12*Lower.dat!B25*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.452528285493532</v>
       </c>
       <c r="C25">
-        <f>4+-12*Lower.dat!B25*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.593225935286675</v>
+        <f>4+-12*Lower.dat!B25*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.983355484906031</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -5195,12 +5195,12 @@
         <v>54.872371200000003</v>
       </c>
       <c r="B26">
-        <f>12*Lower.dat!B26*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8106115203208404</v>
+        <f>12*Lower.dat!B26*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.453695310235315</v>
       </c>
       <c r="C26">
-        <f>4+-12*Lower.dat!B26*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.592475801555651</v>
+        <f>4+-12*Lower.dat!B26*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.982104004089123</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -5209,12 +5209,12 @@
         <v>55.145898000000003</v>
       </c>
       <c r="B27">
-        <f>12*Lower.dat!B27*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8144600160067021</v>
+        <f>12*Lower.dat!B27*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.456615520663131</v>
       </c>
       <c r="C27">
-        <f>4+-12*Lower.dat!B27*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.590598764792702</v>
+        <f>4+-12*Lower.dat!B27*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.978972461799639</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -5223,12 +5223,12 @@
         <v>55.423755599999993</v>
       </c>
       <c r="B28">
-        <f>12*Lower.dat!B28*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8205212139344349</v>
+        <f>12*Lower.dat!B28*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.461214713396718</v>
       </c>
       <c r="C28">
-        <f>4+-12*Lower.dat!B28*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.587642521037601</v>
+        <f>4+-12*Lower.dat!B28*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.974040431420772</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -5237,12 +5237,12 @@
         <v>55.705294800000004</v>
       </c>
       <c r="B29">
-        <f>12*Lower.dat!B29*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8286854450592882</v>
+        <f>12*Lower.dat!B29*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.467409672365626</v>
       </c>
       <c r="C29">
-        <f>4+-12*Lower.dat!B29*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.583660559457424</v>
+        <f>4+-12*Lower.dat!B29*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.967397151262627</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -5251,12 +5251,12 @@
         <v>55.989857999999998</v>
       </c>
       <c r="B30">
-        <f>12*Lower.dat!B30*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8388354809536862</v>
+        <f>12*Lower.dat!B30*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.475111445494917</v>
       </c>
       <c r="C30">
-        <f>4+-12*Lower.dat!B30*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.578710056176615</v>
+        <f>4+-12*Lower.dat!B30*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.959138010747065</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -5265,12 +5265,12 @@
         <v>56.276780400000007</v>
       </c>
       <c r="B31">
-        <f>12*Lower.dat!B31*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8508443780604935</v>
+        <f>12*Lower.dat!B31*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.484223708940281</v>
       </c>
       <c r="C31">
-        <f>4+-12*Lower.dat!B31*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.57285292570489</v>
+        <f>4+-12*Lower.dat!B31*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.949366304550757</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -5279,12 +5279,12 @@
         <v>56.565391199999993</v>
       </c>
       <c r="B32">
-        <f>12*Lower.dat!B32*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8645787147105564</v>
+        <f>12*Lower.dat!B32*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.494645223313299</v>
       </c>
       <c r="C32">
-        <f>4+-12*Lower.dat!B32*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.566154242138317</v>
+        <f>4+-12*Lower.dat!B32*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.938190598626061</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -5293,12 +5293,12 @@
         <v>56.855017200000006</v>
       </c>
       <c r="B33">
-        <f>12*Lower.dat!B33*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8799018308582047</v>
+        <f>12*Lower.dat!B33*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.506272291969097</v>
       </c>
       <c r="C33">
-        <f>4+-12*Lower.dat!B33*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.558680659034732</v>
+        <f>4+-12*Lower.dat!B33*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.925722094010275</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -5307,12 +5307,12 @@
         <v>57.144982799999994</v>
       </c>
       <c r="B34">
-        <f>12*Lower.dat!B34*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.8966738280812452</v>
+        <f>12*Lower.dat!B34*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.51899876100634</v>
       </c>
       <c r="C34">
-        <f>4+-12*Lower.dat!B34*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.550500409413718</v>
+        <f>4+-12*Lower.dat!B34*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.912074626825635</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -5321,12 +5321,12 @@
         <v>57.434608800000007</v>
       </c>
       <c r="B35">
-        <f>12*Lower.dat!B35*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9147537253277029</v>
+        <f>12*Lower.dat!B35*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.532717655032123</v>
       </c>
       <c r="C35">
-        <f>4+-12*Lower.dat!B35*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.541682254328698</v>
+        <f>4+-12*Lower.dat!B35*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.897362914136242</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -5335,12 +5335,12 @@
         <v>57.723219599999993</v>
       </c>
       <c r="B36">
-        <f>12*Lower.dat!B36*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9340005456225278</v>
+        <f>12*Lower.dat!B36*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.547322001747077</v>
       </c>
       <c r="C36">
-        <f>4+-12*Lower.dat!B36*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.532294952844641</v>
+        <f>4+-12*Lower.dat!B36*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.881701669688773</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -5349,12 +5349,12 @@
         <v>58.010143200000002</v>
       </c>
       <c r="B37">
-        <f>12*Lower.dat!B37*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9542733160676047</v>
+        <f>12*Lower.dat!B37*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.562704831945378</v>
       </c>
       <c r="C37">
-        <f>4+-12*Lower.dat!B37*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.522407262038065</v>
+        <f>4+-12*Lower.dat!B37*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.865205603912489</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -5363,12 +5363,12 @@
         <v>58.294705199999996</v>
       </c>
       <c r="B38">
-        <f>12*Lower.dat!B38*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.9754353752582832</v>
+        <f>12*Lower.dat!B38*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.578762447950975</v>
       </c>
       <c r="C38">
-        <f>4+-12*Lower.dat!B38*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.512085836129611</v>
+        <f>4+-12*Lower.dat!B38*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.847985918950499</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -5377,12 +5377,12 @@
         <v>58.576244400000007</v>
       </c>
       <c r="B39">
-        <f>12*Lower.dat!B39*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>6.997351155291514</v>
+        <f>12*Lower.dat!B39*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.59539198182884</v>
       </c>
       <c r="C39">
-        <f>4+-12*Lower.dat!B39*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.501396796003561</v>
+        <f>4+-12*Lower.dat!B39*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.830152927157581</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -5391,12 +5391,12 @@
         <v>58.854101999999997</v>
       </c>
       <c r="B40">
-        <f>12*Lower.dat!B40*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0198883266407659</v>
+        <f>12*Lower.dat!B40*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.612493022900402</v>
       </c>
       <c r="C40">
-        <f>4+-12*Lower.dat!B40*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.490404683082438</v>
+        <f>4+-12*Lower.dat!B40*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.81181430580359</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -5405,12 +5405,12 @@
         <v>59.127629999999996</v>
       </c>
       <c r="B41">
-        <f>12*Lower.dat!B41*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0429178076688661</v>
+        <f>12*Lower.dat!B41*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.629967624961825</v>
       </c>
       <c r="C41">
-        <f>4+-12*Lower.dat!B41*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.479172454687276</v>
+        <f>4+-12*Lower.dat!B41*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.793075089332788</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -5419,12 +5419,12 @@
         <v>59.396187600000005</v>
       </c>
       <c r="B42">
-        <f>12*Lower.dat!B42*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0663126819982089</v>
+        <f>12*Lower.dat!B42*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.647719484792425</v>
       </c>
       <c r="C42">
-        <f>4+-12*Lower.dat!B42*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.467762012071454</v>
+        <f>4+-12*Lower.dat!B42*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.774038550305711</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -5433,12 +5433,12 @@
         <v>59.659149600000006</v>
       </c>
       <c r="B43">
-        <f>12*Lower.dat!B43*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.0899525222350199</v>
+        <f>12*Lower.dat!B43*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.665657222965066</v>
       </c>
       <c r="C43">
-        <f>4+-12*Lower.dat!B43*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.456232091599468</v>
+        <f>4+-12*Lower.dat!B43*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.754802681160751</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -5447,12 +5447,12 @@
         <v>59.915900399999998</v>
       </c>
       <c r="B44">
-        <f>12*Lower.dat!B44*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1137169118573382</v>
+        <f>12*Lower.dat!B44*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.683689468302074</v>
       </c>
       <c r="C44">
-        <f>4+-12*Lower.dat!B44*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.444641424333287</v>
+        <f>4+-12*Lower.dat!B44*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.735465465489856</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -5461,12 +5461,12 @@
         <v>60.165842400000002</v>
       </c>
       <c r="B45">
-        <f>12*Lower.dat!B45*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1374897689392736</v>
+        <f>12*Lower.dat!B45*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.701728138685613</v>
       </c>
       <c r="C45">
-        <f>4+-12*Lower.dat!B45*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.433046627211109</v>
+        <f>4+-12*Lower.dat!B45*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.716121359800098</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -5475,12 +5475,12 @@
         <v>60.408388799999997</v>
       </c>
       <c r="B46">
-        <f>12*Lower.dat!B46*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1611550237857236</v>
+        <f>12*Lower.dat!B46*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.719685161278495</v>
       </c>
       <c r="C46">
-        <f>4+-12*Lower.dat!B46*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.42150431120578</v>
+        <f>4+-12*Lower.dat!B46*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.696864810646289</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -5489,12 +5489,12 @@
         <v>60.6429756</v>
       </c>
       <c r="B47">
-        <f>12*Lower.dat!B47*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.1845998681807091</v>
+        <f>12*Lower.dat!B47*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.737474938030061</v>
       </c>
       <c r="C47">
-        <f>4+-12*Lower.dat!B47*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.410069496560489</v>
+        <f>4+-12*Lower.dat!B47*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.677787610699582</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -5503,12 +5503,12 @@
         <v>60.869053199999996</v>
       </c>
       <c r="B48">
-        <f>12*Lower.dat!B48*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2077158244273924</v>
+        <f>12*Lower.dat!B48*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.755015156855976</v>
       </c>
       <c r="C48">
-        <f>4+-12*Lower.dat!B48*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.398795091383118</v>
+        <f>4+-12*Lower.dat!B48*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.658978028863686</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -5517,12 +5517,12 @@
         <v>61.086094799999998</v>
       </c>
       <c r="B49">
-        <f>12*Lower.dat!B49*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2303901264380706</v>
+        <f>12*Lower.dat!B49*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.772220251672209</v>
       </c>
       <c r="C49">
-        <f>4+-12*Lower.dat!B49*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.387736095369526</v>
+        <f>4+-12*Lower.dat!B49*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.640527823529752</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -5531,12 +5531,12 @@
         <v>61.293593999999999</v>
       </c>
       <c r="B50">
-        <f>12*Lower.dat!B50*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2525154239919161</v>
+        <f>12*Lower.dat!B50*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.789008765914986</v>
       </c>
       <c r="C50">
-        <f>4+-12*Lower.dat!B50*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.376944866720798</v>
+        <f>4+-12*Lower.dat!B50*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.622524346167992</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -5545,12 +5545,12 @@
         <v>61.491064800000004</v>
       </c>
       <c r="B51">
-        <f>12*Lower.dat!B51*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2739843899707086</v>
+        <f>12*Lower.dat!B51*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.805299260550619</v>
       </c>
       <c r="C51">
-        <f>4+-12*Lower.dat!B51*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.36647375237013</v>
+        <f>4+-12*Lower.dat!B51*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.605054929449913</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -5559,12 +5559,12 @@
         <v>61.678046399999999</v>
       </c>
       <c r="B52">
-        <f>12*Lower.dat!B52*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.2946908043475887</v>
+        <f>12*Lower.dat!B52*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.821011136598255</v>
       </c>
       <c r="C52">
-        <f>4+-12*Lower.dat!B52*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.356374559286177</v>
+        <f>4+-12*Lower.dat!B52*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.588206005200643</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -5573,12 +5573,12 @@
         <v>61.854101999999997</v>
       </c>
       <c r="B53">
-        <f>12*Lower.dat!B53*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3145284742752299</v>
+        <f>12*Lower.dat!B53*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.83606381570068</v>
       </c>
       <c r="C53">
-        <f>4+-12*Lower.dat!B53*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.346699081181256</v>
+        <f>4+-12*Lower.dat!B53*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.572063983129159</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -5587,12 +5587,12 @@
         <v>62.018821200000005</v>
       </c>
       <c r="B54">
-        <f>12*Lower.dat!B54*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3333955510152133</v>
+        <f>12*Lower.dat!B54*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.8503800157788</v>
       </c>
       <c r="C54">
-        <f>4+-12*Lower.dat!B54*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.337496993004191</v>
+        <f>4+-12*Lower.dat!B54*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.556711738118931</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -5601,12 +5601,12 @@
         <v>62.171818799999997</v>
       </c>
       <c r="B55">
-        <f>12*Lower.dat!B55*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3511902143676284</v>
+        <f>12*Lower.dat!B55*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.863882476408332</v>
       </c>
       <c r="C55">
-        <f>4+-12*Lower.dat!B55*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.328817955784661</v>
+        <f>4+-12*Lower.dat!B55*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.542232121831482</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -5615,12 +5615,12 @@
         <v>62.312736000000001</v>
       </c>
       <c r="B56">
-        <f>12*Lower.dat!B56*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3678171453471837</v>
+        <f>12*Lower.dat!B56*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.876498870239178</v>
       </c>
       <c r="C56">
-        <f>4+-12*Lower.dat!B56*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.320708459698096</v>
+        <f>4+-12*Lower.dat!B56*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.528702695853934</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -5629,12 +5629,12 @@
         <v>62.441246399999997</v>
       </c>
       <c r="B57">
-        <f>12*Lower.dat!B57*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3831799831080991</v>
+        <f>12*Lower.dat!B57*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.888156079365107</v>
       </c>
       <c r="C57">
-        <f>4+-12*Lower.dat!B57*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.313215503069248</v>
+        <f>4+-12*Lower.dat!B57*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.516201869541071</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -5643,12 +5643,12 @@
         <v>62.557047600000004</v>
       </c>
       <c r="B58">
-        <f>12*Lower.dat!B58*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.3971921009598276</v>
+        <f>12*Lower.dat!B58*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.898788372085814</v>
       </c>
       <c r="C58">
-        <f>4+-12*Lower.dat!B58*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.306381336558132</v>
+        <f>4+-12*Lower.dat!B58*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.504800131511562</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -5657,12 +5657,12 @@
         <v>62.659870799999993</v>
       </c>
       <c r="B59">
-        <f>12*Lower.dat!B59*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4097690673688765</v>
+        <f>12*Lower.dat!B59*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.908331682370136</v>
       </c>
       <c r="C59">
-        <f>4+-12*Lower.dat!B59*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.300247140175141</v>
+        <f>4+-12*Lower.dat!B59*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.494566184172601</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -5671,12 +5671,12 @@
         <v>62.749474800000002</v>
       </c>
       <c r="B60">
-        <f>12*Lower.dat!B60*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4208351104810628</v>
+        <f>12*Lower.dat!B60*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.916728515088337</v>
       </c>
       <c r="C60">
-        <f>4+-12*Lower.dat!B60*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.294849870322853</v>
+        <f>4+-12*Lower.dat!B60*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.485561683502286</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -5685,12 +5685,12 @@
         <v>62.825650800000005</v>
       </c>
       <c r="B61">
-        <f>12*Lower.dat!B61*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4303209664517009</v>
+        <f>12*Lower.dat!B61*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.92392631334079</v>
       </c>
       <c r="C61">
-        <f>4+-12*Lower.dat!B61*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.290223309235532</v>
+        <f>4+-12*Lower.dat!B61*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.477842989875292</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -5699,12 +5699,12 @@
         <v>62.888220000000004</v>
       </c>
       <c r="B62">
-        <f>12*Lower.dat!B62*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4381671123862221</v>
+        <f>12*Lower.dat!B62*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.929879911589673</v>
       </c>
       <c r="C62">
-        <f>4+-12*Lower.dat!B62*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.28639648816862</v>
+        <f>4+-12*Lower.dat!B62*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.47145853740113</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -5713,12 +5713,12 @@
         <v>62.937038400000006</v>
       </c>
       <c r="B63">
-        <f>12*Lower.dat!B63*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4443237717760793</v>
+        <f>12*Lower.dat!B63*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.934551539783733</v>
       </c>
       <c r="C63">
-        <f>4+-12*Lower.dat!B63*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.283393684747487</v>
+        <f>4+-12*Lower.dat!B63*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.466448829500948</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -5727,12 +5727,12 @@
         <v>62.971989600000001</v>
       </c>
       <c r="B64">
-        <f>12*Lower.dat!B64*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4487509063448867</v>
+        <f>12*Lower.dat!B64*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.937910817171179</v>
       </c>
       <c r="C64">
-        <f>4+-12*Lower.dat!B64*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.281234426944316</v>
+        <f>4+-12*Lower.dat!B64*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.462846445542358</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -5741,12 +5741,12 @@
         <v>62.992993200000001</v>
       </c>
       <c r="B65">
-        <f>12*Lower.dat!B65*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4514182255612571</v>
+        <f>12*Lower.dat!B65*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.939934759517946</v>
       </c>
       <c r="C65">
-        <f>4+-12*Lower.dat!B65*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.279933488438381</v>
+        <f>4+-12*Lower.dat!B65*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.460676033098792</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -5755,12 +5755,12 @@
         <v>63</v>
       </c>
       <c r="B66">
-        <f>12*Lower.dat!B66*COS(RADIANS(26))+17*SIN(RADIANS(26))</f>
-        <v>7.4523094954143154</v>
+        <f>12*Lower.dat!B66*COS(RADIANS(47))+30*SIN(RADIANS(47))</f>
+        <v>21.940611048575114</v>
       </c>
       <c r="C66">
-        <f>4+-12*Lower.dat!B66*SIN(RADIANS(26))+17*COS(RADIANS(26))</f>
-        <v>19.279498787085842</v>
+        <f>4+-12*Lower.dat!B66*SIN(RADIANS(47))+30*COS(RADIANS(47))</f>
+        <v>24.459950801874953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>